<commit_message>
removed text pos bias
</commit_message>
<xml_diff>
--- a/CodePad Features.xlsx
+++ b/CodePad Features.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="368">
   <si>
     <t>Feature</t>
   </si>
@@ -947,9 +947,6 @@
     <t>scrolls to visible</t>
   </si>
   <si>
-    <t>wrapped mode: toggles leading at wrap boundary</t>
-  </si>
-  <si>
     <t>caret at the end</t>
   </si>
   <si>
@@ -975,9 +972,6 @@
   </si>
   <si>
     <t>uses phantom position</t>
-  </si>
-  <si>
-    <t>tailing bias at the end of the wrapped row</t>
   </si>
   <si>
     <t>clamp to valid position</t>
@@ -1390,7 +1384,7 @@
           <c:yMode val="edge"/>
           <c:x val="3.8461559098965002E-2"/>
           <c:y val="2.2690437601296611E-2"/>
-          <c:w val="0.91978071330955613"/>
+          <c:w val="0.91978071330955624"/>
           <c:h val="0.89627228525119951"/>
         </c:manualLayout>
       </c:layout>
@@ -1464,7 +1458,7 @@
                   <c:v>292</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>303</c:v>
+                  <c:v>298</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1698,11 +1692,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="174448000"/>
-        <c:axId val="174265472"/>
+        <c:axId val="175431040"/>
+        <c:axId val="175182976"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="174448000"/>
+        <c:axId val="175431040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1735,7 +1729,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="174265472"/>
+        <c:crossAx val="175182976"/>
         <c:crosses val="autoZero"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
@@ -1745,7 +1739,7 @@
         <c:minorTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="174265472"/>
+        <c:axId val="175182976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1787,7 +1781,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="174448000"/>
+        <c:crossAx val="175431040"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1810,7 +1804,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="4.5828229804607823E-2"/>
-          <c:y val="0.33819556996218664"/>
+          <c:y val="0.33819556996218675"/>
           <c:w val="0.12857154394162268"/>
           <c:h val="0.11669367909238262"/>
         </c:manualLayout>
@@ -1914,8 +1908,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.3785273643863572"/>
-          <c:y val="0.13936449433182557"/>
+          <c:x val="0.37852736438635731"/>
+          <c:y val="0.13936449433182563"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -1931,7 +1925,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.4510450248128025E-2"/>
+          <c:x val="4.4510450248128046E-2"/>
           <c:y val="0.10032394165889739"/>
           <c:w val="0.79228601441663349"/>
           <c:h val="0.79935527708863363"/>
@@ -2007,17 +2001,17 @@
                   <c:v>0.70023980815347719</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.72315035799522676</c:v>
+                  <c:v>0.71980676328502413</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="174297472"/>
-        <c:axId val="174299008"/>
+        <c:axId val="175214976"/>
+        <c:axId val="175216512"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="174297472"/>
+        <c:axId val="175214976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2025,13 +2019,13 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy-mm-dd" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="174299008"/>
+        <c:crossAx val="175216512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="174299008"/>
+        <c:axId val="175216512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2074,7 +2068,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="174297472"/>
+        <c:crossAx val="175214976"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2295,11 +2289,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="174987520"/>
-        <c:axId val="174993408"/>
+        <c:axId val="175839488"/>
+        <c:axId val="175845376"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="174987520"/>
+        <c:axId val="175839488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2332,7 +2326,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="174993408"/>
+        <c:crossAx val="175845376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -2341,7 +2335,7 @@
         <c:minorTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="174993408"/>
+        <c:axId val="175845376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2383,7 +2377,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="174987520"/>
+        <c:crossAx val="175839488"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2890,10 +2884,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D514"/>
+  <dimension ref="A1:D509"/>
   <sheetViews>
-    <sheetView topLeftCell="A341" workbookViewId="0">
-      <selection activeCell="D389" sqref="D389"/>
+    <sheetView topLeftCell="A414" workbookViewId="0">
+      <selection activeCell="B445" sqref="B445"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3849,7 +3843,7 @@
     </row>
     <row r="119" spans="2:4" s="38" customFormat="1">
       <c r="B119" s="39" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C119" s="40" t="s">
         <v>14</v>
@@ -3885,7 +3879,7 @@
     </row>
     <row r="123" spans="2:4" s="38" customFormat="1">
       <c r="B123" s="39" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C123" s="40" t="s">
         <v>14</v>
@@ -3921,7 +3915,7 @@
     </row>
     <row r="127" spans="2:4" s="38" customFormat="1">
       <c r="B127" s="39" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C127" s="40" t="s">
         <v>14</v>
@@ -3930,7 +3924,7 @@
     </row>
     <row r="128" spans="2:4" s="38" customFormat="1">
       <c r="B128" s="39" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C128" s="40" t="s">
         <v>2</v>
@@ -3948,7 +3942,7 @@
     </row>
     <row r="130" spans="2:4" s="38" customFormat="1">
       <c r="B130" s="39" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C130" s="40" t="s">
         <v>14</v>
@@ -3984,7 +3978,7 @@
     </row>
     <row r="134" spans="2:4" s="38" customFormat="1">
       <c r="B134" s="39" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C134" s="40" t="s">
         <v>14</v>
@@ -3993,7 +3987,7 @@
     </row>
     <row r="135" spans="2:4" s="38" customFormat="1">
       <c r="B135" s="39" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C135" s="40" t="s">
         <v>14</v>
@@ -4002,7 +3996,7 @@
     </row>
     <row r="136" spans="2:4" s="38" customFormat="1">
       <c r="B136" s="39" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C136" s="40" t="s">
         <v>2</v>
@@ -4020,7 +4014,7 @@
     </row>
     <row r="138" spans="2:4" s="38" customFormat="1">
       <c r="B138" s="39" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C138" s="40" t="s">
         <v>14</v>
@@ -4029,7 +4023,7 @@
     </row>
     <row r="139" spans="2:4" s="38" customFormat="1">
       <c r="B139" s="39" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C139" s="40" t="s">
         <v>14</v>
@@ -4056,7 +4050,7 @@
     </row>
     <row r="142" spans="2:4" s="38" customFormat="1">
       <c r="B142" s="39" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C142" s="40" t="s">
         <v>14</v>
@@ -4065,7 +4059,7 @@
     </row>
     <row r="143" spans="2:4" s="38" customFormat="1">
       <c r="B143" s="39" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C143" s="40" t="s">
         <v>14</v>
@@ -4092,7 +4086,7 @@
     </row>
     <row r="146" spans="2:4" s="38" customFormat="1">
       <c r="B146" s="39" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C146" s="40" t="s">
         <v>14</v>
@@ -4101,7 +4095,7 @@
     </row>
     <row r="147" spans="2:4" s="38" customFormat="1">
       <c r="B147" s="39" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C147" s="40" t="s">
         <v>14</v>
@@ -4153,7 +4147,7 @@
     </row>
     <row r="153" spans="2:4" s="38" customFormat="1">
       <c r="B153" s="39" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C153" s="40" t="s">
         <v>14</v>
@@ -4207,7 +4201,7 @@
     </row>
     <row r="159" spans="2:4" s="38" customFormat="1">
       <c r="B159" s="39" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C159" s="40" t="s">
         <v>14</v>
@@ -4243,7 +4237,7 @@
     </row>
     <row r="163" spans="2:4" s="38" customFormat="1">
       <c r="B163" s="39" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C163" s="40" t="s">
         <v>14</v>
@@ -4279,7 +4273,7 @@
     </row>
     <row r="167" spans="2:4" s="38" customFormat="1">
       <c r="B167" s="39" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C167" s="40" t="s">
         <v>14</v>
@@ -4288,7 +4282,7 @@
     </row>
     <row r="168" spans="2:4" s="38" customFormat="1">
       <c r="B168" s="39" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C168" s="40" t="s">
         <v>14</v>
@@ -4315,7 +4309,7 @@
     </row>
     <row r="171" spans="2:4" s="38" customFormat="1">
       <c r="B171" s="39" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C171" s="40" t="s">
         <v>14</v>
@@ -4324,7 +4318,7 @@
     </row>
     <row r="172" spans="2:4" s="38" customFormat="1">
       <c r="B172" s="39" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C172" s="40" t="s">
         <v>14</v>
@@ -4351,7 +4345,7 @@
     </row>
     <row r="175" spans="2:4" s="38" customFormat="1">
       <c r="B175" s="39" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C175" s="40" t="s">
         <v>2</v>
@@ -4360,7 +4354,7 @@
     </row>
     <row r="176" spans="2:4" s="38" customFormat="1">
       <c r="B176" s="39" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C176" s="40" t="s">
         <v>2</v>
@@ -4369,7 +4363,7 @@
     </row>
     <row r="177" spans="2:4" s="38" customFormat="1">
       <c r="B177" s="39" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C177" s="40" t="s">
         <v>2</v>
@@ -4405,7 +4399,7 @@
     </row>
     <row r="181" spans="2:4" s="38" customFormat="1">
       <c r="B181" s="39" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C181" s="40" t="s">
         <v>2</v>
@@ -4414,7 +4408,7 @@
     </row>
     <row r="182" spans="2:4" s="38" customFormat="1">
       <c r="B182" s="39" t="s">
-        <v>308</v>
+        <v>352</v>
       </c>
       <c r="C182" s="40" t="s">
         <v>2</v>
@@ -4423,7 +4417,7 @@
     </row>
     <row r="183" spans="2:4" s="38" customFormat="1">
       <c r="B183" s="39" t="s">
-        <v>354</v>
+        <v>247</v>
       </c>
       <c r="C183" s="40" t="s">
         <v>2</v>
@@ -4431,8 +4425,8 @@
       <c r="D183" s="40"/>
     </row>
     <row r="184" spans="2:4" s="38" customFormat="1">
-      <c r="B184" s="39" t="s">
-        <v>247</v>
+      <c r="B184" s="42" t="s">
+        <v>149</v>
       </c>
       <c r="C184" s="40" t="s">
         <v>2</v>
@@ -4440,8 +4434,8 @@
       <c r="D184" s="40"/>
     </row>
     <row r="185" spans="2:4" s="38" customFormat="1">
-      <c r="B185" s="42" t="s">
-        <v>149</v>
+      <c r="B185" s="39" t="s">
+        <v>307</v>
       </c>
       <c r="C185" s="40" t="s">
         <v>2</v>
@@ -4450,7 +4444,7 @@
     </row>
     <row r="186" spans="2:4" s="38" customFormat="1">
       <c r="B186" s="39" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C186" s="40" t="s">
         <v>2</v>
@@ -4459,7 +4453,7 @@
     </row>
     <row r="187" spans="2:4" s="38" customFormat="1">
       <c r="B187" s="39" t="s">
-        <v>309</v>
+        <v>352</v>
       </c>
       <c r="C187" s="40" t="s">
         <v>2</v>
@@ -4468,7 +4462,7 @@
     </row>
     <row r="188" spans="2:4" s="38" customFormat="1">
       <c r="B188" s="39" t="s">
-        <v>308</v>
+        <v>248</v>
       </c>
       <c r="C188" s="40" t="s">
         <v>2</v>
@@ -4476,8 +4470,8 @@
       <c r="D188" s="40"/>
     </row>
     <row r="189" spans="2:4" s="38" customFormat="1">
-      <c r="B189" s="39" t="s">
-        <v>354</v>
+      <c r="B189" s="42" t="s">
+        <v>151</v>
       </c>
       <c r="C189" s="40" t="s">
         <v>2</v>
@@ -4486,7 +4480,7 @@
     </row>
     <row r="190" spans="2:4" s="38" customFormat="1">
       <c r="B190" s="39" t="s">
-        <v>248</v>
+        <v>341</v>
       </c>
       <c r="C190" s="40" t="s">
         <v>2</v>
@@ -4494,8 +4488,8 @@
       <c r="D190" s="40"/>
     </row>
     <row r="191" spans="2:4" s="38" customFormat="1">
-      <c r="B191" s="42" t="s">
-        <v>151</v>
+      <c r="B191" s="39" t="s">
+        <v>352</v>
       </c>
       <c r="C191" s="40" t="s">
         <v>2</v>
@@ -4504,7 +4498,7 @@
     </row>
     <row r="192" spans="2:4" s="38" customFormat="1">
       <c r="B192" s="39" t="s">
-        <v>343</v>
+        <v>264</v>
       </c>
       <c r="C192" s="40" t="s">
         <v>2</v>
@@ -4513,7 +4507,7 @@
     </row>
     <row r="193" spans="2:4" s="38" customFormat="1">
       <c r="B193" s="39" t="s">
-        <v>354</v>
+        <v>265</v>
       </c>
       <c r="C193" s="40" t="s">
         <v>2</v>
@@ -4521,8 +4515,8 @@
       <c r="D193" s="40"/>
     </row>
     <row r="194" spans="2:4" s="38" customFormat="1">
-      <c r="B194" s="39" t="s">
-        <v>264</v>
+      <c r="B194" s="42" t="s">
+        <v>150</v>
       </c>
       <c r="C194" s="40" t="s">
         <v>2</v>
@@ -4531,7 +4525,7 @@
     </row>
     <row r="195" spans="2:4" s="38" customFormat="1">
       <c r="B195" s="39" t="s">
-        <v>265</v>
+        <v>342</v>
       </c>
       <c r="C195" s="40" t="s">
         <v>2</v>
@@ -4539,8 +4533,8 @@
       <c r="D195" s="40"/>
     </row>
     <row r="196" spans="2:4" s="38" customFormat="1">
-      <c r="B196" s="42" t="s">
-        <v>150</v>
+      <c r="B196" s="39" t="s">
+        <v>352</v>
       </c>
       <c r="C196" s="40" t="s">
         <v>2</v>
@@ -4549,7 +4543,7 @@
     </row>
     <row r="197" spans="2:4" s="38" customFormat="1">
       <c r="B197" s="39" t="s">
-        <v>344</v>
+        <v>269</v>
       </c>
       <c r="C197" s="40" t="s">
         <v>2</v>
@@ -4558,7 +4552,7 @@
     </row>
     <row r="198" spans="2:4" s="38" customFormat="1">
       <c r="B198" s="39" t="s">
-        <v>354</v>
+        <v>270</v>
       </c>
       <c r="C198" s="40" t="s">
         <v>2</v>
@@ -4566,8 +4560,8 @@
       <c r="D198" s="40"/>
     </row>
     <row r="199" spans="2:4" s="38" customFormat="1">
-      <c r="B199" s="39" t="s">
-        <v>269</v>
+      <c r="B199" s="42" t="s">
+        <v>172</v>
       </c>
       <c r="C199" s="40" t="s">
         <v>2</v>
@@ -4576,7 +4570,7 @@
     </row>
     <row r="200" spans="2:4" s="38" customFormat="1">
       <c r="B200" s="39" t="s">
-        <v>270</v>
+        <v>327</v>
       </c>
       <c r="C200" s="40" t="s">
         <v>2</v>
@@ -4584,8 +4578,8 @@
       <c r="D200" s="40"/>
     </row>
     <row r="201" spans="2:4" s="38" customFormat="1">
-      <c r="B201" s="42" t="s">
-        <v>172</v>
+      <c r="B201" s="39" t="s">
+        <v>328</v>
       </c>
       <c r="C201" s="40" t="s">
         <v>2</v>
@@ -4594,7 +4588,7 @@
     </row>
     <row r="202" spans="2:4" s="38" customFormat="1">
       <c r="B202" s="39" t="s">
-        <v>329</v>
+        <v>352</v>
       </c>
       <c r="C202" s="40" t="s">
         <v>2</v>
@@ -4603,7 +4597,7 @@
     </row>
     <row r="203" spans="2:4" s="38" customFormat="1">
       <c r="B203" s="39" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="C203" s="40" t="s">
         <v>2</v>
@@ -4612,7 +4606,7 @@
     </row>
     <row r="204" spans="2:4" s="38" customFormat="1">
       <c r="B204" s="39" t="s">
-        <v>354</v>
+        <v>319</v>
       </c>
       <c r="C204" s="40" t="s">
         <v>2</v>
@@ -4620,8 +4614,8 @@
       <c r="D204" s="40"/>
     </row>
     <row r="205" spans="2:4" s="38" customFormat="1">
-      <c r="B205" s="39" t="s">
-        <v>322</v>
+      <c r="B205" s="42" t="s">
+        <v>171</v>
       </c>
       <c r="C205" s="40" t="s">
         <v>2</v>
@@ -4630,7 +4624,7 @@
     </row>
     <row r="206" spans="2:4" s="38" customFormat="1">
       <c r="B206" s="39" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="C206" s="40" t="s">
         <v>2</v>
@@ -4638,8 +4632,8 @@
       <c r="D206" s="40"/>
     </row>
     <row r="207" spans="2:4" s="38" customFormat="1">
-      <c r="B207" s="42" t="s">
-        <v>171</v>
+      <c r="B207" s="39" t="s">
+        <v>326</v>
       </c>
       <c r="C207" s="40" t="s">
         <v>2</v>
@@ -4648,7 +4642,7 @@
     </row>
     <row r="208" spans="2:4" s="38" customFormat="1">
       <c r="B208" s="39" t="s">
-        <v>327</v>
+        <v>352</v>
       </c>
       <c r="C208" s="40" t="s">
         <v>2</v>
@@ -4657,7 +4651,7 @@
     </row>
     <row r="209" spans="2:4" s="38" customFormat="1">
       <c r="B209" s="39" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="C209" s="40" t="s">
         <v>2</v>
@@ -4666,7 +4660,7 @@
     </row>
     <row r="210" spans="2:4" s="38" customFormat="1">
       <c r="B210" s="39" t="s">
-        <v>354</v>
+        <v>322</v>
       </c>
       <c r="C210" s="40" t="s">
         <v>2</v>
@@ -4674,8 +4668,8 @@
       <c r="D210" s="40"/>
     </row>
     <row r="211" spans="2:4" s="38" customFormat="1">
-      <c r="B211" s="39" t="s">
-        <v>323</v>
+      <c r="B211" s="42" t="s">
+        <v>173</v>
       </c>
       <c r="C211" s="40" t="s">
         <v>2</v>
@@ -4684,7 +4678,7 @@
     </row>
     <row r="212" spans="2:4" s="38" customFormat="1">
       <c r="B212" s="39" t="s">
-        <v>324</v>
+        <v>334</v>
       </c>
       <c r="C212" s="40" t="s">
         <v>2</v>
@@ -4692,8 +4686,8 @@
       <c r="D212" s="40"/>
     </row>
     <row r="213" spans="2:4" s="38" customFormat="1">
-      <c r="B213" s="42" t="s">
-        <v>173</v>
+      <c r="B213" s="39" t="s">
+        <v>352</v>
       </c>
       <c r="C213" s="40" t="s">
         <v>2</v>
@@ -4702,7 +4696,7 @@
     </row>
     <row r="214" spans="2:4" s="38" customFormat="1">
       <c r="B214" s="39" t="s">
-        <v>336</v>
+        <v>278</v>
       </c>
       <c r="C214" s="40" t="s">
         <v>2</v>
@@ -4710,8 +4704,8 @@
       <c r="D214" s="40"/>
     </row>
     <row r="215" spans="2:4" s="38" customFormat="1">
-      <c r="B215" s="39" t="s">
-        <v>354</v>
+      <c r="B215" s="42" t="s">
+        <v>174</v>
       </c>
       <c r="C215" s="40" t="s">
         <v>2</v>
@@ -4720,7 +4714,7 @@
     </row>
     <row r="216" spans="2:4" s="38" customFormat="1">
       <c r="B216" s="39" t="s">
-        <v>278</v>
+        <v>335</v>
       </c>
       <c r="C216" s="40" t="s">
         <v>2</v>
@@ -4728,8 +4722,8 @@
       <c r="D216" s="40"/>
     </row>
     <row r="217" spans="2:4" s="38" customFormat="1">
-      <c r="B217" s="42" t="s">
-        <v>174</v>
+      <c r="B217" s="39" t="s">
+        <v>352</v>
       </c>
       <c r="C217" s="40" t="s">
         <v>2</v>
@@ -4738,7 +4732,7 @@
     </row>
     <row r="218" spans="2:4" s="38" customFormat="1">
       <c r="B218" s="39" t="s">
-        <v>337</v>
+        <v>278</v>
       </c>
       <c r="C218" s="40" t="s">
         <v>2</v>
@@ -4746,26 +4740,26 @@
       <c r="D218" s="40"/>
     </row>
     <row r="219" spans="2:4" s="38" customFormat="1">
-      <c r="B219" s="39" t="s">
-        <v>354</v>
+      <c r="B219" s="42" t="s">
+        <v>283</v>
       </c>
       <c r="C219" s="40" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D219" s="40"/>
     </row>
     <row r="220" spans="2:4" s="38" customFormat="1">
       <c r="B220" s="39" t="s">
-        <v>278</v>
+        <v>340</v>
       </c>
       <c r="C220" s="40" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D220" s="40"/>
     </row>
     <row r="221" spans="2:4" s="38" customFormat="1">
-      <c r="B221" s="42" t="s">
-        <v>283</v>
+      <c r="B221" s="39" t="s">
+        <v>352</v>
       </c>
       <c r="C221" s="40" t="s">
         <v>14</v>
@@ -4774,43 +4768,43 @@
     </row>
     <row r="222" spans="2:4" s="38" customFormat="1">
       <c r="B222" s="39" t="s">
-        <v>342</v>
+        <v>285</v>
       </c>
       <c r="C222" s="40" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D222" s="40"/>
     </row>
     <row r="223" spans="2:4" s="38" customFormat="1">
       <c r="B223" s="39" t="s">
-        <v>354</v>
+        <v>286</v>
       </c>
       <c r="C223" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="D223" s="40"/>
+    </row>
+    <row r="224" spans="2:4" s="38" customFormat="1">
+      <c r="B224" s="42" t="s">
+        <v>284</v>
+      </c>
+      <c r="C224" s="40" t="s">
         <v>14</v>
-      </c>
-      <c r="D223" s="40"/>
-    </row>
-    <row r="224" spans="2:4" s="38" customFormat="1">
-      <c r="B224" s="39" t="s">
-        <v>285</v>
-      </c>
-      <c r="C224" s="40" t="s">
-        <v>2</v>
       </c>
       <c r="D224" s="40"/>
     </row>
     <row r="225" spans="2:4" s="38" customFormat="1">
       <c r="B225" s="39" t="s">
-        <v>286</v>
+        <v>340</v>
       </c>
       <c r="C225" s="40" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D225" s="40"/>
     </row>
     <row r="226" spans="2:4" s="38" customFormat="1">
-      <c r="B226" s="42" t="s">
-        <v>284</v>
+      <c r="B226" s="39" t="s">
+        <v>352</v>
       </c>
       <c r="C226" s="40" t="s">
         <v>14</v>
@@ -4819,25 +4813,25 @@
     </row>
     <row r="227" spans="2:4" s="38" customFormat="1">
       <c r="B227" s="39" t="s">
-        <v>342</v>
+        <v>293</v>
       </c>
       <c r="C227" s="40" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D227" s="40"/>
     </row>
     <row r="228" spans="2:4" s="38" customFormat="1">
       <c r="B228" s="39" t="s">
-        <v>354</v>
+        <v>294</v>
       </c>
       <c r="C228" s="40" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D228" s="40"/>
     </row>
     <row r="229" spans="2:4" s="38" customFormat="1">
-      <c r="B229" s="39" t="s">
-        <v>293</v>
+      <c r="B229" s="42" t="s">
+        <v>152</v>
       </c>
       <c r="C229" s="40" t="s">
         <v>2</v>
@@ -4846,7 +4840,7 @@
     </row>
     <row r="230" spans="2:4" s="38" customFormat="1">
       <c r="B230" s="39" t="s">
-        <v>294</v>
+        <v>347</v>
       </c>
       <c r="C230" s="40" t="s">
         <v>2</v>
@@ -4854,8 +4848,8 @@
       <c r="D230" s="40"/>
     </row>
     <row r="231" spans="2:4" s="38" customFormat="1">
-      <c r="B231" s="42" t="s">
-        <v>152</v>
+      <c r="B231" s="39" t="s">
+        <v>348</v>
       </c>
       <c r="C231" s="40" t="s">
         <v>2</v>
@@ -4864,7 +4858,7 @@
     </row>
     <row r="232" spans="2:4" s="38" customFormat="1">
       <c r="B232" s="39" t="s">
-        <v>349</v>
+        <v>317</v>
       </c>
       <c r="C232" s="40" t="s">
         <v>2</v>
@@ -4873,7 +4867,7 @@
     </row>
     <row r="233" spans="2:4" s="38" customFormat="1">
       <c r="B233" s="39" t="s">
-        <v>350</v>
+        <v>249</v>
       </c>
       <c r="C233" s="40" t="s">
         <v>2</v>
@@ -4881,8 +4875,8 @@
       <c r="D233" s="40"/>
     </row>
     <row r="234" spans="2:4" s="38" customFormat="1">
-      <c r="B234" s="39" t="s">
-        <v>318</v>
+      <c r="B234" s="42" t="s">
+        <v>153</v>
       </c>
       <c r="C234" s="40" t="s">
         <v>2</v>
@@ -4891,7 +4885,7 @@
     </row>
     <row r="235" spans="2:4" s="38" customFormat="1">
       <c r="B235" s="39" t="s">
-        <v>249</v>
+        <v>354</v>
       </c>
       <c r="C235" s="40" t="s">
         <v>2</v>
@@ -4899,8 +4893,8 @@
       <c r="D235" s="40"/>
     </row>
     <row r="236" spans="2:4" s="38" customFormat="1">
-      <c r="B236" s="42" t="s">
-        <v>153</v>
+      <c r="B236" s="39" t="s">
+        <v>317</v>
       </c>
       <c r="C236" s="40" t="s">
         <v>2</v>
@@ -4909,7 +4903,7 @@
     </row>
     <row r="237" spans="2:4" s="38" customFormat="1">
       <c r="B237" s="39" t="s">
-        <v>356</v>
+        <v>297</v>
       </c>
       <c r="C237" s="40" t="s">
         <v>2</v>
@@ -4917,8 +4911,8 @@
       <c r="D237" s="40"/>
     </row>
     <row r="238" spans="2:4" s="38" customFormat="1">
-      <c r="B238" s="39" t="s">
-        <v>318</v>
+      <c r="B238" s="42" t="s">
+        <v>154</v>
       </c>
       <c r="C238" s="40" t="s">
         <v>2</v>
@@ -4927,7 +4921,7 @@
     </row>
     <row r="239" spans="2:4" s="38" customFormat="1">
       <c r="B239" s="39" t="s">
-        <v>297</v>
+        <v>353</v>
       </c>
       <c r="C239" s="40" t="s">
         <v>2</v>
@@ -4935,8 +4929,8 @@
       <c r="D239" s="40"/>
     </row>
     <row r="240" spans="2:4" s="38" customFormat="1">
-      <c r="B240" s="42" t="s">
-        <v>154</v>
+      <c r="B240" s="39" t="s">
+        <v>317</v>
       </c>
       <c r="C240" s="40" t="s">
         <v>2</v>
@@ -4945,7 +4939,7 @@
     </row>
     <row r="241" spans="2:4" s="38" customFormat="1">
       <c r="B241" s="39" t="s">
-        <v>355</v>
+        <v>298</v>
       </c>
       <c r="C241" s="40" t="s">
         <v>2</v>
@@ -4953,71 +4947,71 @@
       <c r="D241" s="40"/>
     </row>
     <row r="242" spans="2:4" s="38" customFormat="1">
-      <c r="B242" s="39" t="s">
-        <v>318</v>
+      <c r="B242" s="42" t="s">
+        <v>155</v>
       </c>
       <c r="C242" s="40" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D242" s="40"/>
     </row>
     <row r="243" spans="2:4" s="38" customFormat="1">
       <c r="B243" s="39" t="s">
-        <v>298</v>
+        <v>340</v>
       </c>
       <c r="C243" s="40" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D243" s="40"/>
     </row>
     <row r="244" spans="2:4" s="38" customFormat="1">
-      <c r="B244" s="42" t="s">
-        <v>155</v>
+      <c r="B244" s="39" t="s">
+        <v>276</v>
       </c>
       <c r="C244" s="40" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D244" s="40"/>
     </row>
     <row r="245" spans="2:4" s="38" customFormat="1">
       <c r="B245" s="39" t="s">
-        <v>342</v>
+        <v>277</v>
       </c>
       <c r="C245" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="D245" s="40"/>
+    </row>
+    <row r="246" spans="2:4" s="38" customFormat="1">
+      <c r="B246" s="42" t="s">
+        <v>175</v>
+      </c>
+      <c r="C246" s="40" t="s">
         <v>14</v>
-      </c>
-      <c r="D245" s="40"/>
-    </row>
-    <row r="246" spans="2:4" s="38" customFormat="1">
-      <c r="B246" s="39" t="s">
-        <v>276</v>
-      </c>
-      <c r="C246" s="40" t="s">
-        <v>2</v>
       </c>
       <c r="D246" s="40"/>
     </row>
     <row r="247" spans="2:4" s="38" customFormat="1">
       <c r="B247" s="39" t="s">
-        <v>277</v>
+        <v>340</v>
       </c>
       <c r="C247" s="40" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D247" s="40"/>
     </row>
     <row r="248" spans="2:4" s="38" customFormat="1">
-      <c r="B248" s="42" t="s">
-        <v>175</v>
+      <c r="B248" s="39" t="s">
+        <v>282</v>
       </c>
       <c r="C248" s="40" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D248" s="40"/>
     </row>
     <row r="249" spans="2:4" s="38" customFormat="1">
-      <c r="B249" s="39" t="s">
-        <v>342</v>
+      <c r="B249" s="42" t="s">
+        <v>156</v>
       </c>
       <c r="C249" s="40" t="s">
         <v>14</v>
@@ -5026,34 +5020,34 @@
     </row>
     <row r="250" spans="2:4" s="38" customFormat="1">
       <c r="B250" s="39" t="s">
-        <v>282</v>
+        <v>340</v>
       </c>
       <c r="C250" s="40" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D250" s="40"/>
     </row>
     <row r="251" spans="2:4" s="38" customFormat="1">
-      <c r="B251" s="42" t="s">
-        <v>156</v>
+      <c r="B251" s="39" t="s">
+        <v>279</v>
       </c>
       <c r="C251" s="40" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D251" s="40"/>
     </row>
     <row r="252" spans="2:4" s="38" customFormat="1">
       <c r="B252" s="39" t="s">
-        <v>342</v>
+        <v>280</v>
       </c>
       <c r="C252" s="40" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D252" s="40"/>
     </row>
     <row r="253" spans="2:4" s="38" customFormat="1">
       <c r="B253" s="39" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="C253" s="40" t="s">
         <v>2</v>
@@ -5061,8 +5055,8 @@
       <c r="D253" s="40"/>
     </row>
     <row r="254" spans="2:4" s="38" customFormat="1">
-      <c r="B254" s="39" t="s">
-        <v>280</v>
+      <c r="B254" s="42" t="s">
+        <v>157</v>
       </c>
       <c r="C254" s="40" t="s">
         <v>2</v>
@@ -5071,7 +5065,7 @@
     </row>
     <row r="255" spans="2:4" s="38" customFormat="1">
       <c r="B255" s="39" t="s">
-        <v>281</v>
+        <v>343</v>
       </c>
       <c r="C255" s="40" t="s">
         <v>2</v>
@@ -5079,8 +5073,8 @@
       <c r="D255" s="40"/>
     </row>
     <row r="256" spans="2:4" s="38" customFormat="1">
-      <c r="B256" s="42" t="s">
-        <v>157</v>
+      <c r="B256" s="39" t="s">
+        <v>352</v>
       </c>
       <c r="C256" s="40" t="s">
         <v>2</v>
@@ -5089,7 +5083,7 @@
     </row>
     <row r="257" spans="2:4" s="38" customFormat="1">
       <c r="B257" s="39" t="s">
-        <v>345</v>
+        <v>243</v>
       </c>
       <c r="C257" s="40" t="s">
         <v>2</v>
@@ -5097,8 +5091,8 @@
       <c r="D257" s="40"/>
     </row>
     <row r="258" spans="2:4" s="38" customFormat="1">
-      <c r="B258" s="39" t="s">
-        <v>354</v>
+      <c r="B258" s="42" t="s">
+        <v>158</v>
       </c>
       <c r="C258" s="40" t="s">
         <v>2</v>
@@ -5107,7 +5101,7 @@
     </row>
     <row r="259" spans="2:4" s="38" customFormat="1">
       <c r="B259" s="39" t="s">
-        <v>243</v>
+        <v>351</v>
       </c>
       <c r="C259" s="40" t="s">
         <v>2</v>
@@ -5115,8 +5109,8 @@
       <c r="D259" s="40"/>
     </row>
     <row r="260" spans="2:4" s="38" customFormat="1">
-      <c r="B260" s="42" t="s">
-        <v>158</v>
+      <c r="B260" s="39" t="s">
+        <v>350</v>
       </c>
       <c r="C260" s="40" t="s">
         <v>2</v>
@@ -5125,7 +5119,7 @@
     </row>
     <row r="261" spans="2:4" s="38" customFormat="1">
       <c r="B261" s="39" t="s">
-        <v>353</v>
+        <v>317</v>
       </c>
       <c r="C261" s="40" t="s">
         <v>2</v>
@@ -5134,7 +5128,7 @@
     </row>
     <row r="262" spans="2:4" s="38" customFormat="1">
       <c r="B262" s="39" t="s">
-        <v>352</v>
+        <v>255</v>
       </c>
       <c r="C262" s="40" t="s">
         <v>2</v>
@@ -5142,8 +5136,8 @@
       <c r="D262" s="40"/>
     </row>
     <row r="263" spans="2:4" s="38" customFormat="1">
-      <c r="B263" s="39" t="s">
-        <v>318</v>
+      <c r="B263" s="42" t="s">
+        <v>159</v>
       </c>
       <c r="C263" s="40" t="s">
         <v>2</v>
@@ -5152,7 +5146,7 @@
     </row>
     <row r="264" spans="2:4" s="38" customFormat="1">
       <c r="B264" s="39" t="s">
-        <v>255</v>
+        <v>306</v>
       </c>
       <c r="C264" s="40" t="s">
         <v>2</v>
@@ -5160,8 +5154,8 @@
       <c r="D264" s="40"/>
     </row>
     <row r="265" spans="2:4" s="38" customFormat="1">
-      <c r="B265" s="42" t="s">
-        <v>159</v>
+      <c r="B265" s="39" t="s">
+        <v>308</v>
       </c>
       <c r="C265" s="40" t="s">
         <v>2</v>
@@ -5170,7 +5164,7 @@
     </row>
     <row r="266" spans="2:4" s="38" customFormat="1">
       <c r="B266" s="39" t="s">
-        <v>306</v>
+        <v>352</v>
       </c>
       <c r="C266" s="40" t="s">
         <v>2</v>
@@ -5179,7 +5173,7 @@
     </row>
     <row r="267" spans="2:4" s="38" customFormat="1">
       <c r="B267" s="39" t="s">
-        <v>309</v>
+        <v>256</v>
       </c>
       <c r="C267" s="40" t="s">
         <v>2</v>
@@ -5187,8 +5181,8 @@
       <c r="D267" s="40"/>
     </row>
     <row r="268" spans="2:4" s="38" customFormat="1">
-      <c r="B268" s="39" t="s">
-        <v>308</v>
+      <c r="B268" s="42" t="s">
+        <v>160</v>
       </c>
       <c r="C268" s="40" t="s">
         <v>2</v>
@@ -5197,7 +5191,7 @@
     </row>
     <row r="269" spans="2:4" s="38" customFormat="1">
       <c r="B269" s="39" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C269" s="40" t="s">
         <v>2</v>
@@ -5206,7 +5200,7 @@
     </row>
     <row r="270" spans="2:4" s="38" customFormat="1">
       <c r="B270" s="39" t="s">
-        <v>256</v>
+        <v>317</v>
       </c>
       <c r="C270" s="40" t="s">
         <v>2</v>
@@ -5214,8 +5208,8 @@
       <c r="D270" s="40"/>
     </row>
     <row r="271" spans="2:4" s="38" customFormat="1">
-      <c r="B271" s="42" t="s">
-        <v>160</v>
+      <c r="B271" s="39" t="s">
+        <v>296</v>
       </c>
       <c r="C271" s="40" t="s">
         <v>2</v>
@@ -5223,8 +5217,8 @@
       <c r="D271" s="40"/>
     </row>
     <row r="272" spans="2:4" s="38" customFormat="1">
-      <c r="B272" s="39" t="s">
-        <v>357</v>
+      <c r="B272" s="42" t="s">
+        <v>161</v>
       </c>
       <c r="C272" s="40" t="s">
         <v>2</v>
@@ -5233,7 +5227,7 @@
     </row>
     <row r="273" spans="2:4" s="38" customFormat="1">
       <c r="B273" s="39" t="s">
-        <v>318</v>
+        <v>353</v>
       </c>
       <c r="C273" s="40" t="s">
         <v>2</v>
@@ -5242,7 +5236,7 @@
     </row>
     <row r="274" spans="2:4" s="38" customFormat="1">
       <c r="B274" s="39" t="s">
-        <v>296</v>
+        <v>317</v>
       </c>
       <c r="C274" s="40" t="s">
         <v>2</v>
@@ -5250,8 +5244,8 @@
       <c r="D274" s="40"/>
     </row>
     <row r="275" spans="2:4" s="38" customFormat="1">
-      <c r="B275" s="42" t="s">
-        <v>161</v>
+      <c r="B275" s="39" t="s">
+        <v>295</v>
       </c>
       <c r="C275" s="40" t="s">
         <v>2</v>
@@ -5259,8 +5253,8 @@
       <c r="D275" s="40"/>
     </row>
     <row r="276" spans="2:4" s="38" customFormat="1">
-      <c r="B276" s="39" t="s">
-        <v>355</v>
+      <c r="B276" s="42" t="s">
+        <v>195</v>
       </c>
       <c r="C276" s="40" t="s">
         <v>2</v>
@@ -5269,7 +5263,7 @@
     </row>
     <row r="277" spans="2:4" s="38" customFormat="1">
       <c r="B277" s="39" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="C277" s="40" t="s">
         <v>2</v>
@@ -5278,7 +5272,7 @@
     </row>
     <row r="278" spans="2:4" s="38" customFormat="1">
       <c r="B278" s="39" t="s">
-        <v>295</v>
+        <v>312</v>
       </c>
       <c r="C278" s="40" t="s">
         <v>2</v>
@@ -5286,8 +5280,8 @@
       <c r="D278" s="40"/>
     </row>
     <row r="279" spans="2:4" s="38" customFormat="1">
-      <c r="B279" s="42" t="s">
-        <v>195</v>
+      <c r="B279" s="39" t="s">
+        <v>309</v>
       </c>
       <c r="C279" s="40" t="s">
         <v>2</v>
@@ -5296,7 +5290,7 @@
     </row>
     <row r="280" spans="2:4" s="38" customFormat="1">
       <c r="B280" s="39" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C280" s="40" t="s">
         <v>2</v>
@@ -5305,7 +5299,7 @@
     </row>
     <row r="281" spans="2:4" s="38" customFormat="1">
       <c r="B281" s="39" t="s">
-        <v>313</v>
+        <v>352</v>
       </c>
       <c r="C281" s="40" t="s">
         <v>2</v>
@@ -5314,7 +5308,7 @@
     </row>
     <row r="282" spans="2:4" s="38" customFormat="1">
       <c r="B282" s="39" t="s">
-        <v>310</v>
+        <v>278</v>
       </c>
       <c r="C282" s="40" t="s">
         <v>2</v>
@@ -5322,8 +5316,8 @@
       <c r="D282" s="40"/>
     </row>
     <row r="283" spans="2:4" s="38" customFormat="1">
-      <c r="B283" s="39" t="s">
-        <v>311</v>
+      <c r="B283" s="42" t="s">
+        <v>162</v>
       </c>
       <c r="C283" s="40" t="s">
         <v>2</v>
@@ -5332,7 +5326,7 @@
     </row>
     <row r="284" spans="2:4" s="38" customFormat="1">
       <c r="B284" s="39" t="s">
-        <v>354</v>
+        <v>307</v>
       </c>
       <c r="C284" s="40" t="s">
         <v>2</v>
@@ -5341,7 +5335,7 @@
     </row>
     <row r="285" spans="2:4" s="38" customFormat="1">
       <c r="B285" s="39" t="s">
-        <v>278</v>
+        <v>308</v>
       </c>
       <c r="C285" s="40" t="s">
         <v>2</v>
@@ -5349,8 +5343,8 @@
       <c r="D285" s="40"/>
     </row>
     <row r="286" spans="2:4" s="38" customFormat="1">
-      <c r="B286" s="42" t="s">
-        <v>162</v>
+      <c r="B286" s="39" t="s">
+        <v>352</v>
       </c>
       <c r="C286" s="40" t="s">
         <v>2</v>
@@ -5359,7 +5353,7 @@
     </row>
     <row r="287" spans="2:4" s="38" customFormat="1">
       <c r="B287" s="39" t="s">
-        <v>307</v>
+        <v>257</v>
       </c>
       <c r="C287" s="40" t="s">
         <v>2</v>
@@ -5367,8 +5361,8 @@
       <c r="D287" s="40"/>
     </row>
     <row r="288" spans="2:4" s="38" customFormat="1">
-      <c r="B288" s="39" t="s">
-        <v>309</v>
+      <c r="B288" s="42" t="s">
+        <v>176</v>
       </c>
       <c r="C288" s="40" t="s">
         <v>2</v>
@@ -5377,7 +5371,7 @@
     </row>
     <row r="289" spans="2:4" s="38" customFormat="1">
       <c r="B289" s="39" t="s">
-        <v>308</v>
+        <v>344</v>
       </c>
       <c r="C289" s="40" t="s">
         <v>2</v>
@@ -5386,7 +5380,7 @@
     </row>
     <row r="290" spans="2:4" s="38" customFormat="1">
       <c r="B290" s="39" t="s">
-        <v>354</v>
+        <v>271</v>
       </c>
       <c r="C290" s="40" t="s">
         <v>2</v>
@@ -5395,7 +5389,7 @@
     </row>
     <row r="291" spans="2:4" s="38" customFormat="1">
       <c r="B291" s="39" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
       <c r="C291" s="40" t="s">
         <v>2</v>
@@ -5404,7 +5398,7 @@
     </row>
     <row r="292" spans="2:4" s="38" customFormat="1">
       <c r="B292" s="42" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C292" s="40" t="s">
         <v>2</v>
@@ -5413,7 +5407,7 @@
     </row>
     <row r="293" spans="2:4" s="38" customFormat="1">
       <c r="B293" s="39" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C293" s="40" t="s">
         <v>2</v>
@@ -5422,7 +5416,7 @@
     </row>
     <row r="294" spans="2:4" s="38" customFormat="1">
       <c r="B294" s="39" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C294" s="40" t="s">
         <v>2</v>
@@ -5431,7 +5425,7 @@
     </row>
     <row r="295" spans="2:4" s="38" customFormat="1">
       <c r="B295" s="39" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="C295" s="40" t="s">
         <v>2</v>
@@ -5440,7 +5434,7 @@
     </row>
     <row r="296" spans="2:4" s="38" customFormat="1">
       <c r="B296" s="42" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C296" s="40" t="s">
         <v>2</v>
@@ -5449,7 +5443,7 @@
     </row>
     <row r="297" spans="2:4" s="38" customFormat="1">
       <c r="B297" s="39" t="s">
-        <v>347</v>
+        <v>329</v>
       </c>
       <c r="C297" s="40" t="s">
         <v>2</v>
@@ -5458,7 +5452,7 @@
     </row>
     <row r="298" spans="2:4" s="38" customFormat="1">
       <c r="B298" s="39" t="s">
-        <v>272</v>
+        <v>330</v>
       </c>
       <c r="C298" s="40" t="s">
         <v>2</v>
@@ -5467,7 +5461,7 @@
     </row>
     <row r="299" spans="2:4" s="38" customFormat="1">
       <c r="B299" s="39" t="s">
-        <v>273</v>
+        <v>323</v>
       </c>
       <c r="C299" s="40" t="s">
         <v>2</v>
@@ -5475,8 +5469,8 @@
       <c r="D299" s="40"/>
     </row>
     <row r="300" spans="2:4" s="38" customFormat="1">
-      <c r="B300" s="42" t="s">
-        <v>178</v>
+      <c r="B300" s="39" t="s">
+        <v>324</v>
       </c>
       <c r="C300" s="40" t="s">
         <v>2</v>
@@ -5484,8 +5478,8 @@
       <c r="D300" s="40"/>
     </row>
     <row r="301" spans="2:4" s="38" customFormat="1">
-      <c r="B301" s="39" t="s">
-        <v>331</v>
+      <c r="B301" s="42" t="s">
+        <v>179</v>
       </c>
       <c r="C301" s="40" t="s">
         <v>2</v>
@@ -5494,7 +5488,7 @@
     </row>
     <row r="302" spans="2:4" s="38" customFormat="1">
       <c r="B302" s="39" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C302" s="40" t="s">
         <v>2</v>
@@ -5503,7 +5497,7 @@
     </row>
     <row r="303" spans="2:4" s="38" customFormat="1">
       <c r="B303" s="39" t="s">
-        <v>325</v>
+        <v>332</v>
       </c>
       <c r="C303" s="40" t="s">
         <v>2</v>
@@ -5512,7 +5506,7 @@
     </row>
     <row r="304" spans="2:4" s="38" customFormat="1">
       <c r="B304" s="39" t="s">
-        <v>326</v>
+        <v>275</v>
       </c>
       <c r="C304" s="40" t="s">
         <v>2</v>
@@ -5520,8 +5514,8 @@
       <c r="D304" s="40"/>
     </row>
     <row r="305" spans="2:4" s="38" customFormat="1">
-      <c r="B305" s="42" t="s">
-        <v>179</v>
+      <c r="B305" s="39" t="s">
+        <v>274</v>
       </c>
       <c r="C305" s="40" t="s">
         <v>2</v>
@@ -5529,8 +5523,8 @@
       <c r="D305" s="40"/>
     </row>
     <row r="306" spans="2:4" s="38" customFormat="1">
-      <c r="B306" s="39" t="s">
-        <v>333</v>
+      <c r="B306" s="42" t="s">
+        <v>336</v>
       </c>
       <c r="C306" s="40" t="s">
         <v>2</v>
@@ -5539,7 +5533,7 @@
     </row>
     <row r="307" spans="2:4" s="38" customFormat="1">
       <c r="B307" s="39" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="C307" s="40" t="s">
         <v>2</v>
@@ -5548,16 +5542,16 @@
     </row>
     <row r="308" spans="2:4" s="38" customFormat="1">
       <c r="B308" s="39" t="s">
-        <v>275</v>
+        <v>352</v>
       </c>
       <c r="C308" s="40" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D308" s="40"/>
     </row>
     <row r="309" spans="2:4" s="38" customFormat="1">
       <c r="B309" s="39" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="C309" s="40" t="s">
         <v>2</v>
@@ -5566,7 +5560,7 @@
     </row>
     <row r="310" spans="2:4" s="38" customFormat="1">
       <c r="B310" s="42" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C310" s="40" t="s">
         <v>2</v>
@@ -5575,7 +5569,7 @@
     </row>
     <row r="311" spans="2:4" s="38" customFormat="1">
       <c r="B311" s="39" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C311" s="40" t="s">
         <v>2</v>
@@ -5584,7 +5578,7 @@
     </row>
     <row r="312" spans="2:4" s="38" customFormat="1">
       <c r="B312" s="39" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C312" s="40" t="s">
         <v>14</v>
@@ -5602,7 +5596,7 @@
     </row>
     <row r="314" spans="2:4" s="38" customFormat="1">
       <c r="B314" s="42" t="s">
-        <v>339</v>
+        <v>163</v>
       </c>
       <c r="C314" s="40" t="s">
         <v>2</v>
@@ -5611,7 +5605,7 @@
     </row>
     <row r="315" spans="2:4" s="38" customFormat="1">
       <c r="B315" s="39" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="C315" s="40" t="s">
         <v>2</v>
@@ -5620,16 +5614,16 @@
     </row>
     <row r="316" spans="2:4" s="38" customFormat="1">
       <c r="B316" s="39" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="C316" s="40" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D316" s="40"/>
     </row>
     <row r="317" spans="2:4" s="38" customFormat="1">
       <c r="B317" s="39" t="s">
-        <v>278</v>
+        <v>317</v>
       </c>
       <c r="C317" s="40" t="s">
         <v>2</v>
@@ -5637,8 +5631,8 @@
       <c r="D317" s="40"/>
     </row>
     <row r="318" spans="2:4" s="38" customFormat="1">
-      <c r="B318" s="42" t="s">
-        <v>163</v>
+      <c r="B318" s="39" t="s">
+        <v>258</v>
       </c>
       <c r="C318" s="40" t="s">
         <v>2</v>
@@ -5646,26 +5640,26 @@
       <c r="D318" s="40"/>
     </row>
     <row r="319" spans="2:4" s="38" customFormat="1">
-      <c r="B319" s="39" t="s">
-        <v>349</v>
+      <c r="B319" s="42" t="s">
+        <v>196</v>
       </c>
       <c r="C319" s="40" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D319" s="40"/>
     </row>
     <row r="320" spans="2:4" s="38" customFormat="1">
       <c r="B320" s="39" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="C320" s="40" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D320" s="40"/>
     </row>
     <row r="321" spans="2:4" s="38" customFormat="1">
       <c r="B321" s="39" t="s">
-        <v>318</v>
+        <v>278</v>
       </c>
       <c r="C321" s="40" t="s">
         <v>2</v>
@@ -5673,17 +5667,17 @@
       <c r="D321" s="40"/>
     </row>
     <row r="322" spans="2:4" s="38" customFormat="1">
-      <c r="B322" s="39" t="s">
-        <v>258</v>
+      <c r="B322" s="42" t="s">
+        <v>287</v>
       </c>
       <c r="C322" s="40" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D322" s="40"/>
     </row>
     <row r="323" spans="2:4" s="38" customFormat="1">
-      <c r="B323" s="42" t="s">
-        <v>196</v>
+      <c r="B323" s="39" t="s">
+        <v>340</v>
       </c>
       <c r="C323" s="40" t="s">
         <v>14</v>
@@ -5692,16 +5686,16 @@
     </row>
     <row r="324" spans="2:4" s="38" customFormat="1">
       <c r="B324" s="39" t="s">
-        <v>342</v>
+        <v>289</v>
       </c>
       <c r="C324" s="40" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D324" s="40"/>
     </row>
     <row r="325" spans="2:4" s="38" customFormat="1">
       <c r="B325" s="39" t="s">
-        <v>278</v>
+        <v>288</v>
       </c>
       <c r="C325" s="40" t="s">
         <v>2</v>
@@ -5710,7 +5704,7 @@
     </row>
     <row r="326" spans="2:4" s="38" customFormat="1">
       <c r="B326" s="42" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="C326" s="40" t="s">
         <v>14</v>
@@ -5719,7 +5713,7 @@
     </row>
     <row r="327" spans="2:4" s="38" customFormat="1">
       <c r="B327" s="39" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C327" s="40" t="s">
         <v>14</v>
@@ -5728,7 +5722,7 @@
     </row>
     <row r="328" spans="2:4" s="38" customFormat="1">
       <c r="B328" s="39" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C328" s="40" t="s">
         <v>2</v>
@@ -5737,7 +5731,7 @@
     </row>
     <row r="329" spans="2:4" s="38" customFormat="1">
       <c r="B329" s="39" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="C329" s="40" t="s">
         <v>2</v>
@@ -5746,7 +5740,7 @@
     </row>
     <row r="330" spans="2:4" s="38" customFormat="1">
       <c r="B330" s="42" t="s">
-        <v>290</v>
+        <v>164</v>
       </c>
       <c r="C330" s="40" t="s">
         <v>14</v>
@@ -5755,7 +5749,7 @@
     </row>
     <row r="331" spans="2:4" s="38" customFormat="1">
       <c r="B331" s="39" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C331" s="40" t="s">
         <v>14</v>
@@ -5764,7 +5758,7 @@
     </row>
     <row r="332" spans="2:4" s="38" customFormat="1">
       <c r="B332" s="39" t="s">
-        <v>291</v>
+        <v>250</v>
       </c>
       <c r="C332" s="40" t="s">
         <v>2</v>
@@ -5773,7 +5767,7 @@
     </row>
     <row r="333" spans="2:4" s="38" customFormat="1">
       <c r="B333" s="39" t="s">
-        <v>292</v>
+        <v>251</v>
       </c>
       <c r="C333" s="40" t="s">
         <v>2</v>
@@ -5781,44 +5775,34 @@
       <c r="D333" s="40"/>
     </row>
     <row r="334" spans="2:4" s="38" customFormat="1">
-      <c r="B334" s="42" t="s">
-        <v>164</v>
-      </c>
-      <c r="C334" s="40" t="s">
-        <v>14</v>
-      </c>
+      <c r="B334" s="41"/>
+      <c r="C334" s="40"/>
       <c r="D334" s="40"/>
     </row>
     <row r="335" spans="2:4" s="38" customFormat="1">
-      <c r="B335" s="39" t="s">
-        <v>342</v>
-      </c>
-      <c r="C335" s="40" t="s">
-        <v>14</v>
-      </c>
+      <c r="B335" s="41"/>
+      <c r="C335" s="40"/>
       <c r="D335" s="40"/>
     </row>
     <row r="336" spans="2:4" s="38" customFormat="1">
-      <c r="B336" s="39" t="s">
-        <v>250</v>
-      </c>
-      <c r="C336" s="40" t="s">
-        <v>2</v>
-      </c>
+      <c r="B336" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="C336" s="40"/>
       <c r="D336" s="40"/>
     </row>
     <row r="337" spans="2:4" s="38" customFormat="1">
-      <c r="B337" s="39" t="s">
-        <v>251</v>
-      </c>
-      <c r="C337" s="40" t="s">
-        <v>2</v>
-      </c>
+      <c r="B337" s="41"/>
+      <c r="C337" s="40"/>
       <c r="D337" s="40"/>
     </row>
     <row r="338" spans="2:4" s="38" customFormat="1">
-      <c r="B338" s="41"/>
-      <c r="C338" s="40"/>
+      <c r="B338" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="C338" s="40" t="s">
+        <v>2</v>
+      </c>
       <c r="D338" s="40"/>
     </row>
     <row r="339" spans="2:4" s="38" customFormat="1">
@@ -5827,20 +5811,26 @@
       <c r="D339" s="40"/>
     </row>
     <row r="340" spans="2:4" s="38" customFormat="1">
-      <c r="B340" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="C340" s="40"/>
+      <c r="B340" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="C340" s="40" t="s">
+        <v>2</v>
+      </c>
       <c r="D340" s="40"/>
     </row>
     <row r="341" spans="2:4" s="38" customFormat="1">
-      <c r="B341" s="41"/>
-      <c r="C341" s="40"/>
+      <c r="B341" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="C341" s="40" t="s">
+        <v>2</v>
+      </c>
       <c r="D341" s="40"/>
     </row>
     <row r="342" spans="2:4" s="38" customFormat="1">
-      <c r="B342" s="41" t="s">
-        <v>82</v>
+      <c r="B342" s="43" t="s">
+        <v>313</v>
       </c>
       <c r="C342" s="40" t="s">
         <v>2</v>
@@ -5848,13 +5838,17 @@
       <c r="D342" s="40"/>
     </row>
     <row r="343" spans="2:4" s="38" customFormat="1">
-      <c r="B343" s="41"/>
-      <c r="C343" s="40"/>
+      <c r="B343" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="C343" s="40" t="s">
+        <v>14</v>
+      </c>
       <c r="D343" s="40"/>
     </row>
     <row r="344" spans="2:4" s="38" customFormat="1">
-      <c r="B344" s="42" t="s">
-        <v>27</v>
+      <c r="B344" s="39" t="s">
+        <v>314</v>
       </c>
       <c r="C344" s="40" t="s">
         <v>2</v>
@@ -5862,17 +5856,13 @@
       <c r="D344" s="40"/>
     </row>
     <row r="345" spans="2:4" s="38" customFormat="1">
-      <c r="B345" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="C345" s="40" t="s">
-        <v>2</v>
-      </c>
+      <c r="B345" s="39"/>
+      <c r="C345" s="40"/>
       <c r="D345" s="40"/>
     </row>
     <row r="346" spans="2:4" s="38" customFormat="1">
-      <c r="B346" s="43" t="s">
-        <v>314</v>
+      <c r="B346" s="39" t="s">
+        <v>29</v>
       </c>
       <c r="C346" s="40" t="s">
         <v>2</v>
@@ -5880,31 +5870,31 @@
       <c r="D346" s="40"/>
     </row>
     <row r="347" spans="2:4" s="38" customFormat="1">
-      <c r="B347" s="39" t="s">
-        <v>54</v>
+      <c r="B347" s="43" t="s">
+        <v>315</v>
       </c>
       <c r="C347" s="40" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D347" s="40"/>
     </row>
     <row r="348" spans="2:4" s="38" customFormat="1">
-      <c r="B348" s="39" t="s">
-        <v>315</v>
-      </c>
-      <c r="C348" s="40" t="s">
-        <v>2</v>
-      </c>
+      <c r="B348" s="41"/>
+      <c r="C348" s="40"/>
       <c r="D348" s="40"/>
     </row>
     <row r="349" spans="2:4" s="38" customFormat="1">
-      <c r="B349" s="39"/>
-      <c r="C349" s="40"/>
+      <c r="B349" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="C349" s="40" t="s">
+        <v>2</v>
+      </c>
       <c r="D349" s="40"/>
     </row>
     <row r="350" spans="2:4" s="38" customFormat="1">
-      <c r="B350" s="39" t="s">
-        <v>29</v>
+      <c r="B350" s="43" t="s">
+        <v>78</v>
       </c>
       <c r="C350" s="40" t="s">
         <v>2</v>
@@ -5912,22 +5902,22 @@
       <c r="D350" s="40"/>
     </row>
     <row r="351" spans="2:4" s="38" customFormat="1">
-      <c r="B351" s="43" t="s">
+      <c r="B351" s="39"/>
+      <c r="C351" s="40"/>
+      <c r="D351" s="40"/>
+    </row>
+    <row r="352" spans="2:4" s="38" customFormat="1">
+      <c r="B352" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="C352" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="D352" s="40"/>
+    </row>
+    <row r="353" spans="2:4" s="38" customFormat="1">
+      <c r="B353" s="43" t="s">
         <v>316</v>
-      </c>
-      <c r="C351" s="40" t="s">
-        <v>2</v>
-      </c>
-      <c r="D351" s="40"/>
-    </row>
-    <row r="352" spans="2:4" s="38" customFormat="1">
-      <c r="B352" s="41"/>
-      <c r="C352" s="40"/>
-      <c r="D352" s="40"/>
-    </row>
-    <row r="353" spans="2:4" s="38" customFormat="1">
-      <c r="B353" s="39" t="s">
-        <v>36</v>
       </c>
       <c r="C353" s="40" t="s">
         <v>2</v>
@@ -5936,39 +5926,39 @@
     </row>
     <row r="354" spans="2:4" s="38" customFormat="1">
       <c r="B354" s="43" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="C354" s="40" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D354" s="40"/>
     </row>
     <row r="355" spans="2:4" s="38" customFormat="1">
-      <c r="B355" s="39"/>
-      <c r="C355" s="40"/>
+      <c r="B355" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="C355" s="40" t="s">
+        <v>14</v>
+      </c>
       <c r="D355" s="40"/>
     </row>
     <row r="356" spans="2:4" s="38" customFormat="1">
-      <c r="B356" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="C356" s="40" t="s">
-        <v>2</v>
-      </c>
+      <c r="B356" s="41"/>
+      <c r="C356" s="40"/>
       <c r="D356" s="40"/>
     </row>
     <row r="357" spans="2:4" s="38" customFormat="1">
-      <c r="B357" s="43" t="s">
-        <v>317</v>
+      <c r="B357" s="39" t="s">
+        <v>38</v>
       </c>
       <c r="C357" s="40" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D357" s="40"/>
     </row>
     <row r="358" spans="2:4" s="38" customFormat="1">
       <c r="B358" s="43" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C358" s="40" t="s">
         <v>14</v>
@@ -5977,7 +5967,7 @@
     </row>
     <row r="359" spans="2:4" s="38" customFormat="1">
       <c r="B359" s="43" t="s">
-        <v>91</v>
+        <v>52</v>
       </c>
       <c r="C359" s="40" t="s">
         <v>14</v>
@@ -5985,22 +5975,22 @@
       <c r="D359" s="40"/>
     </row>
     <row r="360" spans="2:4" s="38" customFormat="1">
-      <c r="B360" s="41"/>
-      <c r="C360" s="40"/>
+      <c r="B360" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="C360" s="40" t="s">
+        <v>14</v>
+      </c>
       <c r="D360" s="40"/>
     </row>
     <row r="361" spans="2:4" s="38" customFormat="1">
-      <c r="B361" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="C361" s="40" t="s">
-        <v>14</v>
-      </c>
+      <c r="B361" s="41"/>
+      <c r="C361" s="40"/>
       <c r="D361" s="40"/>
     </row>
     <row r="362" spans="2:4" s="38" customFormat="1">
-      <c r="B362" s="43" t="s">
-        <v>40</v>
+      <c r="B362" s="39" t="s">
+        <v>39</v>
       </c>
       <c r="C362" s="40" t="s">
         <v>14</v>
@@ -6009,7 +5999,7 @@
     </row>
     <row r="363" spans="2:4" s="38" customFormat="1">
       <c r="B363" s="43" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="C363" s="40" t="s">
         <v>14</v>
@@ -6017,31 +6007,27 @@
       <c r="D363" s="40"/>
     </row>
     <row r="364" spans="2:4" s="38" customFormat="1">
-      <c r="B364" s="43" t="s">
-        <v>91</v>
-      </c>
-      <c r="C364" s="40" t="s">
-        <v>14</v>
-      </c>
+      <c r="B364" s="41"/>
+      <c r="C364" s="40"/>
       <c r="D364" s="40"/>
     </row>
     <row r="365" spans="2:4" s="38" customFormat="1">
-      <c r="B365" s="41"/>
-      <c r="C365" s="40"/>
+      <c r="B365" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="C365" s="40" t="s">
+        <v>2</v>
+      </c>
       <c r="D365" s="40"/>
     </row>
     <row r="366" spans="2:4" s="38" customFormat="1">
-      <c r="B366" s="39" t="s">
-        <v>39</v>
-      </c>
-      <c r="C366" s="40" t="s">
-        <v>14</v>
-      </c>
+      <c r="B366" s="39"/>
+      <c r="C366" s="40"/>
       <c r="D366" s="40"/>
     </row>
     <row r="367" spans="2:4" s="38" customFormat="1">
-      <c r="B367" s="43" t="s">
-        <v>79</v>
+      <c r="B367" s="42" t="s">
+        <v>28</v>
       </c>
       <c r="C367" s="40" t="s">
         <v>14</v>
@@ -6049,59 +6035,63 @@
       <c r="D367" s="40"/>
     </row>
     <row r="368" spans="2:4" s="38" customFormat="1">
-      <c r="B368" s="41"/>
-      <c r="C368" s="40"/>
+      <c r="B368" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="C368" s="40" t="s">
+        <v>14</v>
+      </c>
       <c r="D368" s="40"/>
     </row>
     <row r="369" spans="2:4" s="38" customFormat="1">
-      <c r="B369" s="39" t="s">
-        <v>42</v>
+      <c r="B369" s="43" t="s">
+        <v>80</v>
       </c>
       <c r="C369" s="40" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D369" s="40"/>
     </row>
     <row r="370" spans="2:4" s="38" customFormat="1">
-      <c r="B370" s="39"/>
+      <c r="B370" s="41"/>
       <c r="C370" s="40"/>
       <c r="D370" s="40"/>
     </row>
     <row r="371" spans="2:4" s="38" customFormat="1">
-      <c r="B371" s="42" t="s">
-        <v>28</v>
+      <c r="B371" s="39" t="s">
+        <v>363</v>
       </c>
       <c r="C371" s="40" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D371" s="40"/>
     </row>
     <row r="372" spans="2:4" s="38" customFormat="1">
       <c r="B372" s="39" t="s">
-        <v>28</v>
+        <v>364</v>
       </c>
       <c r="C372" s="40" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D372" s="40"/>
     </row>
     <row r="373" spans="2:4" s="38" customFormat="1">
-      <c r="B373" s="43" t="s">
-        <v>80</v>
+      <c r="B373" s="39" t="s">
+        <v>365</v>
       </c>
       <c r="C373" s="40" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D373" s="40"/>
     </row>
     <row r="374" spans="2:4" s="38" customFormat="1">
-      <c r="B374" s="41"/>
+      <c r="B374" s="39"/>
       <c r="C374" s="40"/>
       <c r="D374" s="40"/>
     </row>
     <row r="375" spans="2:4" s="38" customFormat="1">
-      <c r="B375" s="39" t="s">
-        <v>365</v>
+      <c r="B375" s="42" t="s">
+        <v>58</v>
       </c>
       <c r="C375" s="40" t="s">
         <v>2</v>
@@ -6110,7 +6100,7 @@
     </row>
     <row r="376" spans="2:4" s="38" customFormat="1">
       <c r="B376" s="39" t="s">
-        <v>366</v>
+        <v>59</v>
       </c>
       <c r="C376" s="40" t="s">
         <v>2</v>
@@ -6119,98 +6109,98 @@
     </row>
     <row r="377" spans="2:4" s="38" customFormat="1">
       <c r="B377" s="39" t="s">
-        <v>367</v>
+        <v>356</v>
       </c>
       <c r="C377" s="40" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D377" s="40"/>
     </row>
     <row r="378" spans="2:4" s="38" customFormat="1">
-      <c r="B378" s="39"/>
-      <c r="C378" s="40"/>
+      <c r="B378" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="C378" s="40" t="s">
+        <v>14</v>
+      </c>
       <c r="D378" s="40"/>
     </row>
     <row r="379" spans="2:4" s="38" customFormat="1">
-      <c r="B379" s="42" t="s">
-        <v>58</v>
+      <c r="B379" s="39" t="s">
+        <v>60</v>
       </c>
       <c r="C379" s="40" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D379" s="40"/>
     </row>
     <row r="380" spans="2:4" s="38" customFormat="1">
-      <c r="B380" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="C380" s="40" t="s">
-        <v>2</v>
-      </c>
+      <c r="B380" s="39"/>
+      <c r="C380" s="40"/>
       <c r="D380" s="40"/>
     </row>
     <row r="381" spans="2:4" s="38" customFormat="1">
-      <c r="B381" s="39" t="s">
-        <v>358</v>
+      <c r="B381" s="42" t="s">
+        <v>366</v>
       </c>
       <c r="C381" s="40" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D381" s="40"/>
     </row>
     <row r="382" spans="2:4" s="38" customFormat="1">
       <c r="B382" s="39" t="s">
-        <v>61</v>
+        <v>362</v>
       </c>
       <c r="C382" s="40" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D382" s="40"/>
     </row>
     <row r="383" spans="2:4" s="38" customFormat="1">
       <c r="B383" s="39" t="s">
-        <v>60</v>
+        <v>361</v>
       </c>
       <c r="C383" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="D383" s="40"/>
+    </row>
+    <row r="384" spans="2:4" s="38" customFormat="1">
+      <c r="B384" s="39" t="s">
+        <v>367</v>
+      </c>
+      <c r="C384" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="D383" s="40"/>
-    </row>
-    <row r="384" spans="2:4" s="38" customFormat="1">
-      <c r="B384" s="39"/>
-      <c r="C384" s="40"/>
       <c r="D384" s="40"/>
     </row>
     <row r="385" spans="2:4" s="38" customFormat="1">
-      <c r="B385" s="42" t="s">
-        <v>368</v>
-      </c>
-      <c r="C385" s="40" t="s">
-        <v>2</v>
-      </c>
+      <c r="B385" s="39"/>
+      <c r="C385" s="40"/>
       <c r="D385" s="40"/>
     </row>
     <row r="386" spans="2:4" s="38" customFormat="1">
-      <c r="B386" s="39" t="s">
-        <v>364</v>
+      <c r="B386" s="42" t="s">
+        <v>136</v>
       </c>
       <c r="C386" s="40" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D386" s="40"/>
     </row>
     <row r="387" spans="2:4" s="38" customFormat="1">
       <c r="B387" s="39" t="s">
-        <v>363</v>
+        <v>137</v>
       </c>
       <c r="C387" s="40" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D387" s="40"/>
     </row>
     <row r="388" spans="2:4" s="38" customFormat="1">
       <c r="B388" s="39" t="s">
-        <v>369</v>
+        <v>138</v>
       </c>
       <c r="C388" s="40" t="s">
         <v>14</v>
@@ -6218,35 +6208,25 @@
       <c r="D388" s="40"/>
     </row>
     <row r="389" spans="2:4" s="38" customFormat="1">
-      <c r="B389" s="39"/>
+      <c r="B389" s="41"/>
       <c r="C389" s="40"/>
       <c r="D389" s="40"/>
     </row>
     <row r="390" spans="2:4" s="38" customFormat="1">
-      <c r="B390" s="42" t="s">
-        <v>136</v>
-      </c>
-      <c r="C390" s="40" t="s">
-        <v>14</v>
-      </c>
+      <c r="B390" s="41"/>
+      <c r="C390" s="40"/>
       <c r="D390" s="40"/>
     </row>
     <row r="391" spans="2:4" s="38" customFormat="1">
-      <c r="B391" s="39" t="s">
-        <v>137</v>
-      </c>
-      <c r="C391" s="40" t="s">
-        <v>14</v>
-      </c>
+      <c r="B391" s="41"/>
+      <c r="C391" s="40"/>
       <c r="D391" s="40"/>
     </row>
     <row r="392" spans="2:4" s="38" customFormat="1">
-      <c r="B392" s="39" t="s">
-        <v>138</v>
-      </c>
-      <c r="C392" s="40" t="s">
-        <v>14</v>
-      </c>
+      <c r="B392" s="37" t="s">
+        <v>357</v>
+      </c>
+      <c r="C392" s="40"/>
       <c r="D392" s="40"/>
     </row>
     <row r="393" spans="2:4" s="38" customFormat="1">
@@ -6255,20 +6235,30 @@
       <c r="D393" s="40"/>
     </row>
     <row r="394" spans="2:4" s="38" customFormat="1">
-      <c r="B394" s="41"/>
-      <c r="C394" s="40"/>
+      <c r="B394" s="41" t="s">
+        <v>358</v>
+      </c>
+      <c r="C394" s="40" t="s">
+        <v>14</v>
+      </c>
       <c r="D394" s="40"/>
     </row>
     <row r="395" spans="2:4" s="38" customFormat="1">
-      <c r="B395" s="41"/>
-      <c r="C395" s="40"/>
+      <c r="B395" s="41" t="s">
+        <v>359</v>
+      </c>
+      <c r="C395" s="40" t="s">
+        <v>14</v>
+      </c>
       <c r="D395" s="40"/>
     </row>
     <row r="396" spans="2:4" s="38" customFormat="1">
-      <c r="B396" s="37" t="s">
-        <v>359</v>
-      </c>
-      <c r="C396" s="40"/>
+      <c r="B396" s="41" t="s">
+        <v>360</v>
+      </c>
+      <c r="C396" s="40" t="s">
+        <v>14</v>
+      </c>
       <c r="D396" s="40"/>
     </row>
     <row r="397" spans="2:4" s="38" customFormat="1">
@@ -6277,30 +6267,18 @@
       <c r="D397" s="40"/>
     </row>
     <row r="398" spans="2:4" s="38" customFormat="1">
-      <c r="B398" s="41" t="s">
-        <v>360</v>
-      </c>
-      <c r="C398" s="40" t="s">
-        <v>14</v>
-      </c>
+      <c r="B398" s="41"/>
+      <c r="C398" s="40"/>
       <c r="D398" s="40"/>
     </row>
     <row r="399" spans="2:4" s="38" customFormat="1">
-      <c r="B399" s="41" t="s">
-        <v>361</v>
-      </c>
-      <c r="C399" s="40" t="s">
-        <v>14</v>
-      </c>
+      <c r="B399" s="41"/>
+      <c r="C399" s="40"/>
       <c r="D399" s="40"/>
     </row>
     <row r="400" spans="2:4" s="38" customFormat="1">
-      <c r="B400" s="41" t="s">
-        <v>362</v>
-      </c>
-      <c r="C400" s="40" t="s">
-        <v>14</v>
-      </c>
+      <c r="B400" s="41"/>
+      <c r="C400" s="40"/>
       <c r="D400" s="40"/>
     </row>
     <row r="401" spans="2:4" s="38" customFormat="1">
@@ -6349,85 +6327,101 @@
       <c r="D409" s="40"/>
     </row>
     <row r="410" spans="2:4" s="38" customFormat="1">
-      <c r="B410" s="41"/>
+      <c r="B410" s="39"/>
       <c r="C410" s="40"/>
       <c r="D410" s="40"/>
     </row>
-    <row r="411" spans="2:4" s="38" customFormat="1">
-      <c r="B411" s="41"/>
+    <row r="411" spans="2:4">
       <c r="C411" s="40"/>
-      <c r="D411" s="40"/>
-    </row>
-    <row r="412" spans="2:4" s="38" customFormat="1">
-      <c r="B412" s="41"/>
+    </row>
+    <row r="412" spans="2:4">
+      <c r="B412" s="37" t="s">
+        <v>45</v>
+      </c>
       <c r="C412" s="40"/>
-      <c r="D412" s="40"/>
-    </row>
-    <row r="413" spans="2:4" s="38" customFormat="1">
-      <c r="B413" s="41"/>
-      <c r="C413" s="40"/>
-      <c r="D413" s="40"/>
-    </row>
-    <row r="414" spans="2:4" s="38" customFormat="1">
-      <c r="B414" s="39"/>
-      <c r="C414" s="40"/>
-      <c r="D414" s="40"/>
+    </row>
+    <row r="414" spans="2:4">
+      <c r="B414" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="C414" s="40" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="415" spans="2:4">
-      <c r="C415" s="40"/>
+      <c r="B415" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="C415" s="40" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="416" spans="2:4">
-      <c r="B416" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="C416" s="40"/>
+      <c r="B416" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="C416" s="40" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="417" spans="2:4">
+      <c r="B417" s="44"/>
+      <c r="C417" s="40"/>
     </row>
     <row r="418" spans="2:4">
-      <c r="B418" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="C418" s="40" t="s">
+      <c r="C418" s="40"/>
+    </row>
+    <row r="420" spans="2:4" s="38" customFormat="1">
+      <c r="B420" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="C420" s="40"/>
+      <c r="D420" s="40"/>
+    </row>
+    <row r="421" spans="2:4" s="38" customFormat="1">
+      <c r="B421" s="41"/>
+      <c r="C421" s="40"/>
+      <c r="D421" s="40"/>
+    </row>
+    <row r="422" spans="2:4" s="38" customFormat="1">
+      <c r="B422" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="C422" s="40" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="419" spans="2:4">
-      <c r="B419" s="44" t="s">
-        <v>43</v>
-      </c>
-      <c r="C419" s="40" t="s">
+      <c r="D422" s="40"/>
+    </row>
+    <row r="423" spans="2:4" s="38" customFormat="1">
+      <c r="B423" s="41" t="s">
+        <v>131</v>
+      </c>
+      <c r="C423" s="40" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="420" spans="2:4">
-      <c r="B420" s="44" t="s">
-        <v>63</v>
-      </c>
-      <c r="C420" s="40" t="s">
+      <c r="D423" s="40"/>
+    </row>
+    <row r="424" spans="2:4" s="38" customFormat="1">
+      <c r="B424" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="C424" s="40" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="421" spans="2:4">
-      <c r="B421" s="44"/>
-      <c r="C421" s="40"/>
-    </row>
-    <row r="422" spans="2:4">
-      <c r="C422" s="40"/>
-    </row>
-    <row r="424" spans="2:4" s="38" customFormat="1">
-      <c r="B424" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="C424" s="40"/>
       <c r="D424" s="40"/>
     </row>
     <row r="425" spans="2:4" s="38" customFormat="1">
-      <c r="B425" s="41"/>
-      <c r="C425" s="40"/>
+      <c r="B425" s="41" t="s">
+        <v>132</v>
+      </c>
+      <c r="C425" s="40" t="s">
+        <v>14</v>
+      </c>
       <c r="D425" s="40"/>
     </row>
     <row r="426" spans="2:4" s="38" customFormat="1">
       <c r="B426" s="41" t="s">
-        <v>92</v>
+        <v>133</v>
       </c>
       <c r="C426" s="40" t="s">
         <v>14</v>
@@ -6435,17 +6429,13 @@
       <c r="D426" s="40"/>
     </row>
     <row r="427" spans="2:4" s="38" customFormat="1">
-      <c r="B427" s="41" t="s">
-        <v>131</v>
-      </c>
-      <c r="C427" s="40" t="s">
-        <v>14</v>
-      </c>
+      <c r="B427" s="41"/>
+      <c r="C427" s="40"/>
       <c r="D427" s="40"/>
     </row>
     <row r="428" spans="2:4" s="38" customFormat="1">
       <c r="B428" s="41" t="s">
-        <v>130</v>
+        <v>26</v>
       </c>
       <c r="C428" s="40" t="s">
         <v>14</v>
@@ -6453,8 +6443,8 @@
       <c r="D428" s="40"/>
     </row>
     <row r="429" spans="2:4" s="38" customFormat="1">
-      <c r="B429" s="41" t="s">
-        <v>132</v>
+      <c r="B429" s="39" t="s">
+        <v>99</v>
       </c>
       <c r="C429" s="40" t="s">
         <v>14</v>
@@ -6462,8 +6452,8 @@
       <c r="D429" s="40"/>
     </row>
     <row r="430" spans="2:4" s="38" customFormat="1">
-      <c r="B430" s="41" t="s">
-        <v>133</v>
+      <c r="B430" s="39" t="s">
+        <v>97</v>
       </c>
       <c r="C430" s="40" t="s">
         <v>14</v>
@@ -6471,22 +6461,22 @@
       <c r="D430" s="40"/>
     </row>
     <row r="431" spans="2:4" s="38" customFormat="1">
-      <c r="B431" s="41"/>
-      <c r="C431" s="40"/>
+      <c r="B431" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="C431" s="40" t="s">
+        <v>14</v>
+      </c>
       <c r="D431" s="40"/>
     </row>
     <row r="432" spans="2:4" s="38" customFormat="1">
-      <c r="B432" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="C432" s="40" t="s">
-        <v>14</v>
-      </c>
+      <c r="B432" s="39"/>
+      <c r="C432" s="40"/>
       <c r="D432" s="40"/>
     </row>
     <row r="433" spans="2:4" s="38" customFormat="1">
-      <c r="B433" s="39" t="s">
-        <v>99</v>
+      <c r="B433" s="41" t="s">
+        <v>46</v>
       </c>
       <c r="C433" s="40" t="s">
         <v>14</v>
@@ -6494,17 +6484,13 @@
       <c r="D433" s="40"/>
     </row>
     <row r="434" spans="2:4" s="38" customFormat="1">
-      <c r="B434" s="39" t="s">
-        <v>97</v>
-      </c>
-      <c r="C434" s="40" t="s">
-        <v>14</v>
-      </c>
+      <c r="B434" s="41"/>
+      <c r="C434" s="40"/>
       <c r="D434" s="40"/>
     </row>
     <row r="435" spans="2:4" s="38" customFormat="1">
-      <c r="B435" s="39" t="s">
-        <v>98</v>
+      <c r="B435" s="41" t="s">
+        <v>134</v>
       </c>
       <c r="C435" s="40" t="s">
         <v>14</v>
@@ -6512,17 +6498,13 @@
       <c r="D435" s="40"/>
     </row>
     <row r="436" spans="2:4" s="38" customFormat="1">
-      <c r="B436" s="39"/>
+      <c r="B436" s="41"/>
       <c r="C436" s="40"/>
       <c r="D436" s="40"/>
     </row>
     <row r="437" spans="2:4" s="38" customFormat="1">
-      <c r="B437" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="C437" s="40" t="s">
-        <v>14</v>
-      </c>
+      <c r="B437" s="41"/>
+      <c r="C437" s="40"/>
       <c r="D437" s="40"/>
     </row>
     <row r="438" spans="2:4" s="38" customFormat="1">
@@ -6531,12 +6513,10 @@
       <c r="D438" s="40"/>
     </row>
     <row r="439" spans="2:4" s="38" customFormat="1">
-      <c r="B439" s="41" t="s">
-        <v>134</v>
-      </c>
-      <c r="C439" s="40" t="s">
-        <v>14</v>
-      </c>
+      <c r="B439" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="C439" s="40"/>
       <c r="D439" s="40"/>
     </row>
     <row r="440" spans="2:4" s="38" customFormat="1">
@@ -6545,39 +6525,53 @@
       <c r="D440" s="40"/>
     </row>
     <row r="441" spans="2:4" s="38" customFormat="1">
-      <c r="B441" s="41"/>
-      <c r="C441" s="40"/>
+      <c r="B441" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="C441" s="40" t="s">
+        <v>14</v>
+      </c>
       <c r="D441" s="40"/>
     </row>
     <row r="442" spans="2:4" s="38" customFormat="1">
-      <c r="B442" s="41"/>
-      <c r="C442" s="40"/>
+      <c r="B442" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="C442" s="40" t="s">
+        <v>14</v>
+      </c>
       <c r="D442" s="40"/>
     </row>
     <row r="443" spans="2:4" s="38" customFormat="1">
-      <c r="B443" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="C443" s="40"/>
+      <c r="B443" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="C443" s="40" t="s">
+        <v>14</v>
+      </c>
       <c r="D443" s="40"/>
     </row>
     <row r="444" spans="2:4" s="38" customFormat="1">
-      <c r="B444" s="41"/>
-      <c r="C444" s="40"/>
+      <c r="B444" s="41" t="s">
+        <v>126</v>
+      </c>
+      <c r="C444" s="40" t="s">
+        <v>2</v>
+      </c>
       <c r="D444" s="40"/>
     </row>
     <row r="445" spans="2:4" s="38" customFormat="1">
-      <c r="B445" s="41" t="s">
-        <v>96</v>
+      <c r="B445" s="39" t="s">
+        <v>318</v>
       </c>
       <c r="C445" s="40" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D445" s="40"/>
     </row>
     <row r="446" spans="2:4" s="38" customFormat="1">
       <c r="B446" s="41" t="s">
-        <v>94</v>
+        <v>193</v>
       </c>
       <c r="C446" s="40" t="s">
         <v>14</v>
@@ -6586,7 +6580,7 @@
     </row>
     <row r="447" spans="2:4" s="38" customFormat="1">
       <c r="B447" s="41" t="s">
-        <v>95</v>
+        <v>127</v>
       </c>
       <c r="C447" s="40" t="s">
         <v>14</v>
@@ -6595,92 +6589,92 @@
     </row>
     <row r="448" spans="2:4" s="38" customFormat="1">
       <c r="B448" s="41" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C448" s="40" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D448" s="40"/>
     </row>
     <row r="449" spans="2:4" s="38" customFormat="1">
-      <c r="B449" s="39" t="s">
-        <v>320</v>
+      <c r="B449" s="41" t="s">
+        <v>129</v>
       </c>
       <c r="C449" s="40" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D449" s="40"/>
     </row>
     <row r="450" spans="2:4" s="38" customFormat="1">
-      <c r="B450" s="39" t="s">
-        <v>319</v>
-      </c>
-      <c r="C450" s="40" t="s">
-        <v>2</v>
-      </c>
+      <c r="B450" s="41"/>
+      <c r="C450" s="40"/>
       <c r="D450" s="40"/>
     </row>
     <row r="451" spans="2:4" s="38" customFormat="1">
-      <c r="B451" s="41" t="s">
-        <v>193</v>
-      </c>
-      <c r="C451" s="40" t="s">
-        <v>14</v>
-      </c>
+      <c r="B451" s="41"/>
+      <c r="C451" s="40"/>
       <c r="D451" s="40"/>
     </row>
     <row r="452" spans="2:4" s="38" customFormat="1">
-      <c r="B452" s="41" t="s">
-        <v>127</v>
-      </c>
-      <c r="C452" s="40" t="s">
-        <v>14</v>
-      </c>
+      <c r="B452" s="37" t="s">
+        <v>197</v>
+      </c>
+      <c r="C452" s="40"/>
       <c r="D452" s="40"/>
     </row>
     <row r="453" spans="2:4" s="38" customFormat="1">
-      <c r="B453" s="41" t="s">
-        <v>128</v>
-      </c>
-      <c r="C453" s="40" t="s">
-        <v>14</v>
-      </c>
+      <c r="B453" s="41"/>
+      <c r="C453" s="40"/>
       <c r="D453" s="40"/>
     </row>
     <row r="454" spans="2:4" s="38" customFormat="1">
       <c r="B454" s="41" t="s">
-        <v>129</v>
+        <v>198</v>
       </c>
       <c r="C454" s="40" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D454" s="40"/>
     </row>
     <row r="455" spans="2:4" s="38" customFormat="1">
-      <c r="B455" s="41"/>
-      <c r="C455" s="40"/>
+      <c r="B455" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="C455" s="40" t="s">
+        <v>2</v>
+      </c>
       <c r="D455" s="40"/>
     </row>
     <row r="456" spans="2:4" s="38" customFormat="1">
-      <c r="B456" s="41"/>
-      <c r="C456" s="40"/>
+      <c r="B456" s="41" t="s">
+        <v>199</v>
+      </c>
+      <c r="C456" s="40" t="s">
+        <v>2</v>
+      </c>
       <c r="D456" s="40"/>
     </row>
     <row r="457" spans="2:4" s="38" customFormat="1">
-      <c r="B457" s="37" t="s">
-        <v>197</v>
-      </c>
-      <c r="C457" s="40"/>
+      <c r="B457" s="41" t="s">
+        <v>200</v>
+      </c>
+      <c r="C457" s="40" t="s">
+        <v>2</v>
+      </c>
       <c r="D457" s="40"/>
     </row>
     <row r="458" spans="2:4" s="38" customFormat="1">
-      <c r="B458" s="41"/>
-      <c r="C458" s="40"/>
+      <c r="B458" s="41" t="s">
+        <v>201</v>
+      </c>
+      <c r="C458" s="40" t="s">
+        <v>2</v>
+      </c>
       <c r="D458" s="40"/>
     </row>
     <row r="459" spans="2:4" s="38" customFormat="1">
       <c r="B459" s="41" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="C459" s="40" t="s">
         <v>2</v>
@@ -6689,7 +6683,7 @@
     </row>
     <row r="460" spans="2:4" s="38" customFormat="1">
       <c r="B460" s="41" t="s">
-        <v>26</v>
+        <v>203</v>
       </c>
       <c r="C460" s="40" t="s">
         <v>2</v>
@@ -6698,7 +6692,7 @@
     </row>
     <row r="461" spans="2:4" s="38" customFormat="1">
       <c r="B461" s="41" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="C461" s="40" t="s">
         <v>2</v>
@@ -6707,7 +6701,7 @@
     </row>
     <row r="462" spans="2:4" s="38" customFormat="1">
       <c r="B462" s="41" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="C462" s="40" t="s">
         <v>2</v>
@@ -6716,7 +6710,7 @@
     </row>
     <row r="463" spans="2:4" s="38" customFormat="1">
       <c r="B463" s="41" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="C463" s="40" t="s">
         <v>2</v>
@@ -6725,7 +6719,7 @@
     </row>
     <row r="464" spans="2:4" s="38" customFormat="1">
       <c r="B464" s="41" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="C464" s="40" t="s">
         <v>2</v>
@@ -6734,7 +6728,7 @@
     </row>
     <row r="465" spans="2:4" s="38" customFormat="1">
       <c r="B465" s="41" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="C465" s="40" t="s">
         <v>2</v>
@@ -6743,7 +6737,7 @@
     </row>
     <row r="466" spans="2:4" s="38" customFormat="1">
       <c r="B466" s="41" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="C466" s="40" t="s">
         <v>2</v>
@@ -6752,7 +6746,7 @@
     </row>
     <row r="467" spans="2:4" s="38" customFormat="1">
       <c r="B467" s="41" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="C467" s="40" t="s">
         <v>2</v>
@@ -6761,7 +6755,7 @@
     </row>
     <row r="468" spans="2:4" s="38" customFormat="1">
       <c r="B468" s="41" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="C468" s="40" t="s">
         <v>2</v>
@@ -6770,7 +6764,7 @@
     </row>
     <row r="469" spans="2:4" s="38" customFormat="1">
       <c r="B469" s="41" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="C469" s="40" t="s">
         <v>2</v>
@@ -6779,7 +6773,7 @@
     </row>
     <row r="470" spans="2:4" s="38" customFormat="1">
       <c r="B470" s="41" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="C470" s="40" t="s">
         <v>2</v>
@@ -6788,7 +6782,7 @@
     </row>
     <row r="471" spans="2:4" s="38" customFormat="1">
       <c r="B471" s="41" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="C471" s="40" t="s">
         <v>2</v>
@@ -6797,7 +6791,7 @@
     </row>
     <row r="472" spans="2:4" s="38" customFormat="1">
       <c r="B472" s="41" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="C472" s="40" t="s">
         <v>2</v>
@@ -6806,7 +6800,7 @@
     </row>
     <row r="473" spans="2:4" s="38" customFormat="1">
       <c r="B473" s="41" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C473" s="40" t="s">
         <v>2</v>
@@ -6815,7 +6809,7 @@
     </row>
     <row r="474" spans="2:4" s="38" customFormat="1">
       <c r="B474" s="41" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="C474" s="40" t="s">
         <v>2</v>
@@ -6824,7 +6818,7 @@
     </row>
     <row r="475" spans="2:4" s="38" customFormat="1">
       <c r="B475" s="41" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="C475" s="40" t="s">
         <v>2</v>
@@ -6833,7 +6827,7 @@
     </row>
     <row r="476" spans="2:4" s="38" customFormat="1">
       <c r="B476" s="41" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="C476" s="40" t="s">
         <v>2</v>
@@ -6842,7 +6836,7 @@
     </row>
     <row r="477" spans="2:4" s="38" customFormat="1">
       <c r="B477" s="41" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="C477" s="40" t="s">
         <v>2</v>
@@ -6851,7 +6845,7 @@
     </row>
     <row r="478" spans="2:4" s="38" customFormat="1">
       <c r="B478" s="41" t="s">
-        <v>216</v>
+        <v>302</v>
       </c>
       <c r="C478" s="40" t="s">
         <v>2</v>
@@ -6860,7 +6854,7 @@
     </row>
     <row r="479" spans="2:4" s="38" customFormat="1">
       <c r="B479" s="41" t="s">
-        <v>217</v>
+        <v>303</v>
       </c>
       <c r="C479" s="40" t="s">
         <v>2</v>
@@ -6869,7 +6863,7 @@
     </row>
     <row r="480" spans="2:4" s="38" customFormat="1">
       <c r="B480" s="41" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="C480" s="40" t="s">
         <v>2</v>
@@ -6878,7 +6872,7 @@
     </row>
     <row r="481" spans="2:4" s="38" customFormat="1">
       <c r="B481" s="41" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="C481" s="40" t="s">
         <v>2</v>
@@ -6887,7 +6881,7 @@
     </row>
     <row r="482" spans="2:4" s="38" customFormat="1">
       <c r="B482" s="41" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C482" s="40" t="s">
         <v>2</v>
@@ -6896,7 +6890,7 @@
     </row>
     <row r="483" spans="2:4" s="38" customFormat="1">
       <c r="B483" s="41" t="s">
-        <v>302</v>
+        <v>224</v>
       </c>
       <c r="C483" s="40" t="s">
         <v>2</v>
@@ -6905,7 +6899,7 @@
     </row>
     <row r="484" spans="2:4" s="38" customFormat="1">
       <c r="B484" s="41" t="s">
-        <v>303</v>
+        <v>225</v>
       </c>
       <c r="C484" s="40" t="s">
         <v>2</v>
@@ -6914,7 +6908,7 @@
     </row>
     <row r="485" spans="2:4" s="38" customFormat="1">
       <c r="B485" s="41" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="C485" s="40" t="s">
         <v>2</v>
@@ -6923,7 +6917,7 @@
     </row>
     <row r="486" spans="2:4" s="38" customFormat="1">
       <c r="B486" s="41" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="C486" s="40" t="s">
         <v>2</v>
@@ -6932,7 +6926,7 @@
     </row>
     <row r="487" spans="2:4" s="38" customFormat="1">
       <c r="B487" s="41" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="C487" s="40" t="s">
         <v>2</v>
@@ -6941,7 +6935,7 @@
     </row>
     <row r="488" spans="2:4" s="38" customFormat="1">
       <c r="B488" s="41" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="C488" s="40" t="s">
         <v>2</v>
@@ -6950,7 +6944,7 @@
     </row>
     <row r="489" spans="2:4" s="38" customFormat="1">
       <c r="B489" s="41" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="C489" s="40" t="s">
         <v>2</v>
@@ -6959,7 +6953,7 @@
     </row>
     <row r="490" spans="2:4" s="38" customFormat="1">
       <c r="B490" s="41" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="C490" s="40" t="s">
         <v>2</v>
@@ -6968,7 +6962,7 @@
     </row>
     <row r="491" spans="2:4" s="38" customFormat="1">
       <c r="B491" s="41" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="C491" s="40" t="s">
         <v>2</v>
@@ -6977,7 +6971,7 @@
     </row>
     <row r="492" spans="2:4" s="38" customFormat="1">
       <c r="B492" s="41" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="C492" s="40" t="s">
         <v>2</v>
@@ -6986,7 +6980,7 @@
     </row>
     <row r="493" spans="2:4" s="38" customFormat="1">
       <c r="B493" s="41" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="C493" s="40" t="s">
         <v>2</v>
@@ -6995,7 +6989,7 @@
     </row>
     <row r="494" spans="2:4" s="38" customFormat="1">
       <c r="B494" s="41" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="C494" s="40" t="s">
         <v>2</v>
@@ -7004,7 +6998,7 @@
     </row>
     <row r="495" spans="2:4" s="38" customFormat="1">
       <c r="B495" s="41" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="C495" s="40" t="s">
         <v>2</v>
@@ -7013,7 +7007,7 @@
     </row>
     <row r="496" spans="2:4" s="38" customFormat="1">
       <c r="B496" s="41" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="C496" s="40" t="s">
         <v>2</v>
@@ -7022,7 +7016,7 @@
     </row>
     <row r="497" spans="1:4" s="38" customFormat="1">
       <c r="B497" s="41" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="C497" s="40" t="s">
         <v>2</v>
@@ -7031,7 +7025,7 @@
     </row>
     <row r="498" spans="1:4" s="38" customFormat="1">
       <c r="B498" s="41" t="s">
-        <v>234</v>
+        <v>304</v>
       </c>
       <c r="C498" s="40" t="s">
         <v>2</v>
@@ -7040,7 +7034,7 @@
     </row>
     <row r="499" spans="1:4" s="38" customFormat="1">
       <c r="B499" s="41" t="s">
-        <v>235</v>
+        <v>305</v>
       </c>
       <c r="C499" s="40" t="s">
         <v>2</v>
@@ -7049,7 +7043,7 @@
     </row>
     <row r="500" spans="1:4" s="38" customFormat="1">
       <c r="B500" s="41" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="C500" s="40" t="s">
         <v>2</v>
@@ -7057,126 +7051,81 @@
       <c r="D500" s="40"/>
     </row>
     <row r="501" spans="1:4" s="38" customFormat="1">
-      <c r="B501" s="41" t="s">
-        <v>237</v>
-      </c>
-      <c r="C501" s="40" t="s">
-        <v>2</v>
-      </c>
+      <c r="B501" s="41"/>
+      <c r="C501" s="40"/>
       <c r="D501" s="40"/>
     </row>
     <row r="502" spans="1:4" s="38" customFormat="1">
-      <c r="B502" s="41" t="s">
-        <v>238</v>
-      </c>
-      <c r="C502" s="40" t="s">
-        <v>2</v>
-      </c>
+      <c r="B502" s="41"/>
+      <c r="C502" s="40"/>
       <c r="D502" s="40"/>
     </row>
-    <row r="503" spans="1:4" s="38" customFormat="1">
-      <c r="B503" s="41" t="s">
-        <v>304</v>
-      </c>
-      <c r="C503" s="40" t="s">
-        <v>2</v>
-      </c>
-      <c r="D503" s="40"/>
-    </row>
-    <row r="504" spans="1:4" s="38" customFormat="1">
-      <c r="B504" s="41" t="s">
-        <v>305</v>
-      </c>
-      <c r="C504" s="40" t="s">
-        <v>2</v>
-      </c>
-      <c r="D504" s="40"/>
-    </row>
-    <row r="505" spans="1:4" s="38" customFormat="1">
-      <c r="B505" s="41" t="s">
-        <v>239</v>
-      </c>
-      <c r="C505" s="40" t="s">
-        <v>2</v>
-      </c>
-      <c r="D505" s="40"/>
-    </row>
-    <row r="506" spans="1:4" s="38" customFormat="1">
-      <c r="B506" s="41"/>
-      <c r="C506" s="40"/>
-      <c r="D506" s="40"/>
-    </row>
-    <row r="507" spans="1:4" s="38" customFormat="1">
-      <c r="B507" s="41"/>
-      <c r="C507" s="40"/>
-      <c r="D507" s="40"/>
+    <row r="503" spans="1:4">
+      <c r="A503" s="37"/>
+      <c r="B503" s="45"/>
+      <c r="C503" s="45"/>
+      <c r="D503" s="37"/>
+    </row>
+    <row r="504" spans="1:4">
+      <c r="A504" s="37"/>
+      <c r="B504" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="C504" s="38">
+        <f>COUNTIF(C5:C503,"y")</f>
+        <v>298</v>
+      </c>
+    </row>
+    <row r="505" spans="1:4">
+      <c r="A505" s="37"/>
+      <c r="B505" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C505" s="38">
+        <f>COUNTIF(C5:C503,"n")</f>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="506" spans="1:4">
+      <c r="A506" s="37"/>
+      <c r="B506" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="C506" s="40">
+        <f>COUNTIF(C5:C503,"TBD")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="507" spans="1:4">
+      <c r="A507" s="37"/>
+      <c r="B507" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="C507" s="35">
+        <f>SUM(C504:C506)</f>
+        <v>414</v>
+      </c>
     </row>
     <row r="508" spans="1:4">
       <c r="A508" s="37"/>
-      <c r="B508" s="45"/>
-      <c r="C508" s="45"/>
-      <c r="D508" s="37"/>
+      <c r="B508" s="47"/>
+      <c r="C508" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="D508" s="48">
+        <f>C504/(C505+C504 + C506)</f>
+        <v>0.71980676328502413</v>
+      </c>
     </row>
     <row r="509" spans="1:4">
       <c r="A509" s="37"/>
-      <c r="B509" s="46" t="s">
-        <v>6</v>
-      </c>
-      <c r="C509" s="38">
-        <f>COUNTIF(C5:C508,"y")</f>
-        <v>303</v>
-      </c>
-    </row>
-    <row r="510" spans="1:4">
-      <c r="A510" s="37"/>
-      <c r="B510" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="C510" s="38">
-        <f>COUNTIF(C5:C508,"n")</f>
-        <v>116</v>
-      </c>
-    </row>
-    <row r="511" spans="1:4">
-      <c r="A511" s="37"/>
-      <c r="B511" s="46" t="s">
-        <v>3</v>
-      </c>
-      <c r="C511" s="40">
-        <f>COUNTIF(C5:C508,"TBD")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="512" spans="1:4">
-      <c r="A512" s="37"/>
-      <c r="B512" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="C512" s="35">
-        <f>SUM(C509:C511)</f>
-        <v>419</v>
-      </c>
-    </row>
-    <row r="513" spans="1:4">
-      <c r="A513" s="37"/>
-      <c r="B513" s="47"/>
-      <c r="C513" s="47" t="s">
-        <v>5</v>
-      </c>
-      <c r="D513" s="48">
-        <f>C509/(C510+C509 + C511)</f>
-        <v>0.72315035799522676</v>
-      </c>
-    </row>
-    <row r="514" spans="1:4">
-      <c r="A514" s="37"/>
-      <c r="B514" s="45"/>
-      <c r="C514" s="45"/>
-      <c r="D514" s="37"/>
+      <c r="B509" s="45"/>
+      <c r="C509" s="45"/>
+      <c r="D509" s="37"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
-  <conditionalFormatting sqref="C424:C65262 C418:C422 C1:C3 C6:C416">
+  <conditionalFormatting sqref="C420:C65257 C414:C418 C1:C3 C6:C412">
     <cfRule type="cellIs" dxfId="2" priority="19" stopIfTrue="1" operator="equal">
       <formula>"y"</formula>
     </cfRule>
@@ -7203,7 +7152,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="9660" topLeftCell="A46" activePane="bottomLeft"/>
       <selection sqref="A1:XFD1"/>
-      <selection pane="bottomLeft" activeCell="D52" sqref="D52"/>
+      <selection pane="bottomLeft" activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -7539,7 +7488,7 @@
         <v>45665</v>
       </c>
       <c r="B52" s="5">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="C52" s="5">
         <v>116</v>
@@ -7553,7 +7502,7 @@
       <c r="F52" s="17"/>
       <c r="G52" s="14">
         <f t="shared" ref="G52" si="2">B52/SUM(B52:E52)</f>
-        <v>0.72315035799522676</v>
+        <v>0.71980676328502413</v>
       </c>
       <c r="H52" s="5"/>
     </row>
@@ -7596,25 +7545,25 @@
       <c r="F55" s="15"/>
       <c r="G55" s="18">
         <f>MIN(G52)</f>
-        <v>0.72315035799522676</v>
+        <v>0.71980676328502413</v>
       </c>
       <c r="H55" s="5"/>
     </row>
     <row r="56" spans="1:10">
       <c r="A56" s="19">
         <f>SUM(B56:D56)</f>
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="B56" s="20">
-        <f>Features!C509</f>
-        <v>303</v>
+        <f>Features!C504</f>
+        <v>298</v>
       </c>
       <c r="C56" s="21">
-        <f>Features!C510</f>
+        <f>Features!C505</f>
         <v>116</v>
       </c>
       <c r="D56" s="22">
-        <f>Features!C511</f>
+        <f>Features!C506</f>
         <v>0</v>
       </c>
       <c r="E56" s="23">
@@ -7662,7 +7611,7 @@
       </c>
       <c r="B60" s="26">
         <f>(A52-A48)*A56/B56 +A48</f>
-        <v>45686.438943894391</v>
+        <v>45686.798657718122</v>
       </c>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>

</xml_diff>